<commit_message>
DOC updating readme and adding aus tables
</commit_message>
<xml_diff>
--- a/dev/data/survivor-au-confessionals.xlsx
+++ b/dev/data/survivor-au-confessionals.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dan\Google Drive\R Code\my-packages\survivoR\dev\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8002FAF2-E4DB-4E75-A11D-1DF9B9D867C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46058E94-96FF-4C67-936E-A8834589A7A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" activeTab="1" xr2:uid="{22E0698C-8932-416E-AF95-78770299D9ED}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" firstSheet="1" activeTab="1" xr2:uid="{22E0698C-8932-416E-AF95-78770299D9ED}"/>
   </bookViews>
   <sheets>
-    <sheet name="Pivot" sheetId="16" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="17" state="hidden" r:id="rId1"/>
     <sheet name="Confessionals" sheetId="11" r:id="rId2"/>
     <sheet name="Table" sheetId="15" r:id="rId3"/>
   </sheets>
@@ -22,7 +22,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="11" r:id="rId4"/>
+    <pivotCache cacheId="18" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -353,7 +353,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -372,9 +372,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -411,9 +408,9 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Daniel Oehm" refreshedDate="44607.912881828706" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" recordCount="168" xr:uid="{C9BE09F5-5532-430D-B759-6F7A07AC72FA}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Daniel Oehm" refreshedDate="44607.971429050929" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" recordCount="186" xr:uid="{09B81C42-1F32-493D-A094-1828F2ECB888}">
   <cacheSource type="worksheet">
-    <worksheetSource ref="A1:F169" sheet="Confessionals"/>
+    <worksheetSource ref="A1:F187" sheet="Confessionals"/>
   </cacheSource>
   <cacheFields count="6">
     <cacheField name="Season Name" numFmtId="0">
@@ -423,7 +420,7 @@
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="7" maxValue="7"/>
     </cacheField>
     <cacheField name="Episode" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="8" count="8">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="9" count="9">
         <n v="1"/>
         <n v="2"/>
         <n v="3"/>
@@ -432,6 +429,7 @@
         <n v="6"/>
         <n v="7"/>
         <n v="8"/>
+        <n v="9"/>
       </sharedItems>
     </cacheField>
     <cacheField name="Castaway ID" numFmtId="0">
@@ -478,7 +476,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="168">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="186">
   <r>
     <s v="Survivor: Blood V. Water"/>
     <n v="7"/>
@@ -1823,17 +1821,161 @@
     <x v="22"/>
     <n v="0"/>
   </r>
+  <r>
+    <s v="Survivor: Blood V. Water"/>
+    <n v="7"/>
+    <x v="8"/>
+    <s v="AU0001"/>
+    <x v="1"/>
+    <n v="7"/>
+  </r>
+  <r>
+    <s v="Survivor: Blood V. Water"/>
+    <n v="7"/>
+    <x v="8"/>
+    <s v="AU0002"/>
+    <x v="3"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <s v="Survivor: Blood V. Water"/>
+    <n v="7"/>
+    <x v="8"/>
+    <s v="AU0003"/>
+    <x v="6"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <s v="Survivor: Blood V. Water"/>
+    <n v="7"/>
+    <x v="8"/>
+    <s v="AU0004"/>
+    <x v="7"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <s v="Survivor: Blood V. Water"/>
+    <n v="7"/>
+    <x v="8"/>
+    <s v="AU0006"/>
+    <x v="9"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <s v="Survivor: Blood V. Water"/>
+    <n v="7"/>
+    <x v="8"/>
+    <s v="AU0007"/>
+    <x v="10"/>
+    <n v="7"/>
+  </r>
+  <r>
+    <s v="Survivor: Blood V. Water"/>
+    <n v="7"/>
+    <x v="8"/>
+    <s v="AU0009"/>
+    <x v="18"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <s v="Survivor: Blood V. Water"/>
+    <n v="7"/>
+    <x v="8"/>
+    <s v="AU0010"/>
+    <x v="20"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <s v="Survivor: Blood V. Water"/>
+    <n v="7"/>
+    <x v="8"/>
+    <s v="AU0012"/>
+    <x v="23"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <s v="Survivor: Blood V. Water"/>
+    <n v="7"/>
+    <x v="8"/>
+    <s v="AU0016"/>
+    <x v="5"/>
+    <n v="4"/>
+  </r>
+  <r>
+    <s v="Survivor: Blood V. Water"/>
+    <n v="7"/>
+    <x v="8"/>
+    <s v="AU0017"/>
+    <x v="11"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <s v="Survivor: Blood V. Water"/>
+    <n v="7"/>
+    <x v="8"/>
+    <s v="AU0018"/>
+    <x v="12"/>
+    <n v="8"/>
+  </r>
+  <r>
+    <s v="Survivor: Blood V. Water"/>
+    <n v="7"/>
+    <x v="8"/>
+    <s v="AU0019"/>
+    <x v="14"/>
+    <n v="4"/>
+  </r>
+  <r>
+    <s v="Survivor: Blood V. Water"/>
+    <n v="7"/>
+    <x v="8"/>
+    <s v="AU0020"/>
+    <x v="15"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <s v="Survivor: Blood V. Water"/>
+    <n v="7"/>
+    <x v="8"/>
+    <s v="AU0021"/>
+    <x v="16"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <s v="Survivor: Blood V. Water"/>
+    <n v="7"/>
+    <x v="8"/>
+    <s v="AU0022"/>
+    <x v="17"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <s v="Survivor: Blood V. Water"/>
+    <n v="7"/>
+    <x v="8"/>
+    <s v="AU0023"/>
+    <x v="19"/>
+    <n v="7"/>
+  </r>
+  <r>
+    <s v="Survivor: Blood V. Water"/>
+    <n v="7"/>
+    <x v="8"/>
+    <s v="AU0024"/>
+    <x v="22"/>
+    <n v="1"/>
+  </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7E698E5D-3CF6-4894-8205-4F765272EC04}" name="PivotTable3" cacheId="11" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A3:J29" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{63A8B301-3C2E-42ED-A9F3-C8CAD4EC449B}" name="PivotTable5" cacheId="18" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:K29" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField axis="axisCol" showAll="0">
-      <items count="9">
+      <items count="10">
         <item x="0"/>
         <item x="1"/>
         <item x="2"/>
@@ -1842,6 +1984,7 @@
         <item x="5"/>
         <item x="6"/>
         <item x="7"/>
+        <item x="8"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -1960,7 +2103,7 @@
   <colFields count="1">
     <field x="2"/>
   </colFields>
-  <colItems count="9">
+  <colItems count="10">
     <i>
       <x/>
     </i>
@@ -1984,6 +2127,9 @@
     </i>
     <i>
       <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
     </i>
     <i t="grand">
       <x/>
@@ -2300,22 +2446,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A90DA450-F4C8-418D-BDE9-729CF9377BBB}">
-  <dimension ref="A3:J29"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F537B13A-F125-4516-AC8E-0BC38A122EBA}">
+  <dimension ref="A3:K29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+      <selection activeCell="A5" sqref="A5:J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="22.796875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.73046875" bestFit="1" customWidth="1"/>
-    <col min="3" max="9" width="2.73046875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.19921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="10" width="2.73046875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>58</v>
       </c>
@@ -2323,7 +2469,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>55</v>
       </c>
@@ -2351,11 +2497,14 @@
       <c r="I4">
         <v>8</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4">
+        <v>9</v>
+      </c>
+      <c r="K4" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A5" s="3" t="s">
         <v>9</v>
       </c>
@@ -2377,11 +2526,12 @@
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
-      <c r="J5" s="4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J5" s="4"/>
+      <c r="K5" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A6" s="3" t="s">
         <v>16</v>
       </c>
@@ -2410,10 +2560,13 @@
         <v>0</v>
       </c>
       <c r="J6" s="4">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
+        <v>7</v>
+      </c>
+      <c r="K6" s="4">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A7" s="3" t="s">
         <v>4</v>
       </c>
@@ -2427,11 +2580,12 @@
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
-      <c r="J7" s="4">
+      <c r="J7" s="4"/>
+      <c r="K7" s="4">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A8" s="3" t="s">
         <v>8</v>
       </c>
@@ -2460,10 +2614,13 @@
         <v>0</v>
       </c>
       <c r="J8" s="4">
+        <v>0</v>
+      </c>
+      <c r="K8" s="4">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A9" s="3" t="s">
         <v>10</v>
       </c>
@@ -2479,11 +2636,12 @@
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
-      <c r="J9" s="4">
+      <c r="J9" s="4"/>
+      <c r="K9" s="4">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A10" s="3" t="s">
         <v>18</v>
       </c>
@@ -2512,10 +2670,13 @@
         <v>2</v>
       </c>
       <c r="J10" s="4">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
+        <v>4</v>
+      </c>
+      <c r="K10" s="4">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A11" s="3" t="s">
         <v>17</v>
       </c>
@@ -2544,10 +2705,13 @@
         <v>4</v>
       </c>
       <c r="J11" s="4">
+        <v>0</v>
+      </c>
+      <c r="K11" s="4">
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A12" s="3" t="s">
         <v>6</v>
       </c>
@@ -2576,10 +2740,13 @@
         <v>0</v>
       </c>
       <c r="J12" s="4">
+        <v>0</v>
+      </c>
+      <c r="K12" s="4">
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A13" s="3" t="s">
         <v>12</v>
       </c>
@@ -2603,11 +2770,12 @@
       </c>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
-      <c r="J13" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J13" s="4"/>
+      <c r="K13" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A14" s="3" t="s">
         <v>11</v>
       </c>
@@ -2636,10 +2804,13 @@
         <v>0</v>
       </c>
       <c r="J14" s="4">
+        <v>0</v>
+      </c>
+      <c r="K14" s="4">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A15" s="3" t="s">
         <v>21</v>
       </c>
@@ -2668,10 +2839,13 @@
         <v>0</v>
       </c>
       <c r="J15" s="4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
+        <v>7</v>
+      </c>
+      <c r="K15" s="4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A16" s="3" t="s">
         <v>22</v>
       </c>
@@ -2700,10 +2874,13 @@
         <v>3</v>
       </c>
       <c r="J16" s="4">
+        <v>0</v>
+      </c>
+      <c r="K16" s="4">
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A17" s="3" t="s">
         <v>13</v>
       </c>
@@ -2732,10 +2909,13 @@
         <v>0</v>
       </c>
       <c r="J17" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
+        <v>8</v>
+      </c>
+      <c r="K17" s="4">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A18" s="3" t="s">
         <v>20</v>
       </c>
@@ -2753,11 +2933,12 @@
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
-      <c r="J18" s="4">
+      <c r="J18" s="4"/>
+      <c r="K18" s="4">
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A19" s="3" t="s">
         <v>15</v>
       </c>
@@ -2786,10 +2967,13 @@
         <v>0</v>
       </c>
       <c r="J19" s="4">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.45">
+        <v>4</v>
+      </c>
+      <c r="K19" s="4">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A20" s="3" t="s">
         <v>14</v>
       </c>
@@ -2818,10 +3002,13 @@
         <v>4</v>
       </c>
       <c r="J20" s="4">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.45">
+        <v>1</v>
+      </c>
+      <c r="K20" s="4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A21" s="3" t="s">
         <v>23</v>
       </c>
@@ -2850,10 +3037,13 @@
         <v>0</v>
       </c>
       <c r="J21" s="4">
+        <v>0</v>
+      </c>
+      <c r="K21" s="4">
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A22" s="3" t="s">
         <v>19</v>
       </c>
@@ -2884,8 +3074,11 @@
       <c r="J22" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K22" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A23" s="3" t="s">
         <v>3</v>
       </c>
@@ -2914,10 +3107,13 @@
         <v>0</v>
       </c>
       <c r="J23" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.45">
+        <v>0</v>
+      </c>
+      <c r="K23" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A24" s="3" t="s">
         <v>7</v>
       </c>
@@ -2946,10 +3142,13 @@
         <v>2</v>
       </c>
       <c r="J24" s="4">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.45">
+        <v>7</v>
+      </c>
+      <c r="K24" s="4">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A25" s="3" t="s">
         <v>5</v>
       </c>
@@ -2978,10 +3177,13 @@
         <v>7</v>
       </c>
       <c r="J25" s="4">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.45">
+        <v>2</v>
+      </c>
+      <c r="K25" s="4">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A26" s="3" t="s">
         <v>0</v>
       </c>
@@ -3007,11 +3209,12 @@
         <v>4</v>
       </c>
       <c r="I26" s="4"/>
-      <c r="J26" s="4">
+      <c r="J26" s="4"/>
+      <c r="K26" s="4">
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A27" s="3" t="s">
         <v>1</v>
       </c>
@@ -3040,10 +3243,13 @@
         <v>0</v>
       </c>
       <c r="J27" s="4">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.45">
+        <v>1</v>
+      </c>
+      <c r="K27" s="4">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A28" s="3" t="s">
         <v>2</v>
       </c>
@@ -3072,10 +3278,13 @@
         <v>4</v>
       </c>
       <c r="J28" s="4">
+        <v>0</v>
+      </c>
+      <c r="K28" s="4">
         <v>29</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A29" s="3" t="s">
         <v>56</v>
       </c>
@@ -3104,7 +3313,10 @@
         <v>26</v>
       </c>
       <c r="J29" s="4">
-        <v>314</v>
+        <v>41</v>
+      </c>
+      <c r="K29" s="4">
+        <v>355</v>
       </c>
     </row>
   </sheetData>
@@ -3116,8 +3328,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{823259C0-A9B2-4D8C-810E-0A651DDDB32E}">
   <dimension ref="A1:F187"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A134" workbookViewId="0">
-      <selection activeCell="C165" sqref="C165"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -6885,7 +7097,7 @@
   <dimension ref="A1:L27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -6933,949 +7145,1007 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A2" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="6">
-        <v>3</v>
-      </c>
-      <c r="C2" s="6">
-        <v>2</v>
-      </c>
-      <c r="D2" s="6">
+      <c r="A2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="4">
+        <v>3</v>
+      </c>
+      <c r="C2" s="4">
+        <v>2</v>
+      </c>
+      <c r="D2" s="4">
         <v>14</v>
       </c>
-      <c r="E2" s="6">
-        <v>7</v>
-      </c>
-      <c r="F2" s="6">
-        <v>2</v>
-      </c>
-      <c r="G2" s="6">
+      <c r="E2" s="4">
+        <v>7</v>
+      </c>
+      <c r="F2" s="4">
+        <v>2</v>
+      </c>
+      <c r="G2" s="4">
         <v>13</v>
       </c>
-      <c r="H2" s="6">
+      <c r="H2" s="4">
         <v>4</v>
       </c>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
       <c r="K2" s="6">
         <f>SUM(B2:J2)</f>
         <v>45</v>
       </c>
       <c r="L2" s="7">
-        <f>K2/COUNTIF(B2:I2, "&lt;&gt;")</f>
+        <f>K2/COUNTIF(B2:J2, "&lt;&gt;")</f>
         <v>6.4285714285714288</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A3" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="6">
-        <v>2</v>
-      </c>
-      <c r="C3" s="6">
-        <v>3</v>
-      </c>
-      <c r="D3" s="6">
-        <v>0</v>
-      </c>
-      <c r="E3" s="6">
+      <c r="A3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="4">
+        <v>1</v>
+      </c>
+      <c r="C3" s="4">
+        <v>6</v>
+      </c>
+      <c r="D3" s="4">
+        <v>8</v>
+      </c>
+      <c r="E3" s="4">
+        <v>3</v>
+      </c>
+      <c r="F3" s="4">
+        <v>6</v>
+      </c>
+      <c r="G3" s="4">
+        <v>3</v>
+      </c>
+      <c r="H3" s="4">
+        <v>0</v>
+      </c>
+      <c r="I3" s="4">
+        <v>0</v>
+      </c>
+      <c r="J3" s="4">
+        <v>4</v>
+      </c>
+      <c r="K3" s="6">
+        <f>SUM(B3:J3)</f>
+        <v>31</v>
+      </c>
+      <c r="L3" s="7">
+        <f>K3/COUNTIF(B3:J3, "&lt;&gt;")</f>
+        <v>3.4444444444444446</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="4">
+        <v>8</v>
+      </c>
+      <c r="C4" s="4">
+        <v>9</v>
+      </c>
+      <c r="D4" s="4">
+        <v>4</v>
+      </c>
+      <c r="E4" s="4">
+        <v>0</v>
+      </c>
+      <c r="F4" s="4">
+        <v>0</v>
+      </c>
+      <c r="G4" s="4">
+        <v>0</v>
+      </c>
+      <c r="H4" s="4">
+        <v>2</v>
+      </c>
+      <c r="I4" s="4">
+        <v>2</v>
+      </c>
+      <c r="J4" s="4">
+        <v>4</v>
+      </c>
+      <c r="K4" s="6">
+        <f>SUM(B4:J4)</f>
+        <v>29</v>
+      </c>
+      <c r="L4" s="7">
+        <f>K4/COUNTIF(B4:J4, "&lt;&gt;")</f>
+        <v>3.2222222222222223</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="4">
+        <v>2</v>
+      </c>
+      <c r="C5" s="4">
+        <v>3</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0</v>
+      </c>
+      <c r="E5" s="4">
         <v>11</v>
       </c>
-      <c r="F3" s="6">
+      <c r="F5" s="4">
         <v>6</v>
       </c>
-      <c r="G3" s="6">
-        <v>3</v>
-      </c>
-      <c r="H3" s="6">
-        <v>0</v>
-      </c>
-      <c r="I3" s="6">
+      <c r="G5" s="4">
+        <v>3</v>
+      </c>
+      <c r="H5" s="4">
+        <v>0</v>
+      </c>
+      <c r="I5" s="4">
         <v>4</v>
       </c>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6">
-        <f t="shared" ref="K3:K25" si="0">SUM(B3:J3)</f>
+      <c r="J5" s="4">
+        <v>0</v>
+      </c>
+      <c r="K5" s="6">
+        <f>SUM(B5:J5)</f>
         <v>29</v>
       </c>
-      <c r="L3" s="7">
-        <f>K3/COUNTIF(B3:I3, "&lt;&gt;")</f>
-        <v>3.625</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A4" s="9" t="s">
+      <c r="L5" s="7">
+        <f>K5/COUNTIF(B5:J5, "&lt;&gt;")</f>
+        <v>3.2222222222222223</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="4">
+        <v>6</v>
+      </c>
+      <c r="C6" s="4">
+        <v>4</v>
+      </c>
+      <c r="D6" s="4">
+        <v>0</v>
+      </c>
+      <c r="E6" s="4">
+        <v>0</v>
+      </c>
+      <c r="F6" s="4">
+        <v>0</v>
+      </c>
+      <c r="G6" s="4">
+        <v>0</v>
+      </c>
+      <c r="H6" s="4">
+        <v>9</v>
+      </c>
+      <c r="I6" s="4">
+        <v>2</v>
+      </c>
+      <c r="J6" s="4">
+        <v>7</v>
+      </c>
+      <c r="K6" s="6">
+        <f>SUM(B6:J6)</f>
+        <v>28</v>
+      </c>
+      <c r="L6" s="7">
+        <f>K6/COUNTIF(B6:J6, "&lt;&gt;")</f>
+        <v>3.1111111111111112</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A7" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="4">
+        <v>1</v>
+      </c>
+      <c r="C7" s="4">
+        <v>3</v>
+      </c>
+      <c r="D7" s="4">
+        <v>4</v>
+      </c>
+      <c r="E7" s="4">
+        <v>4</v>
+      </c>
+      <c r="F7" s="4">
+        <v>3</v>
+      </c>
+      <c r="G7" s="4">
+        <v>0</v>
+      </c>
+      <c r="H7" s="4">
+        <v>4</v>
+      </c>
+      <c r="I7" s="4">
+        <v>7</v>
+      </c>
+      <c r="J7" s="4">
+        <v>2</v>
+      </c>
+      <c r="K7" s="6">
+        <f>SUM(B7:J7)</f>
+        <v>28</v>
+      </c>
+      <c r="L7" s="7">
+        <f>K7/COUNTIF(B7:J7, "&lt;&gt;")</f>
+        <v>3.1111111111111112</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="4">
+        <v>1</v>
+      </c>
+      <c r="C8" s="4">
+        <v>0</v>
+      </c>
+      <c r="D8" s="4">
+        <v>0</v>
+      </c>
+      <c r="E8" s="4">
+        <v>2</v>
+      </c>
+      <c r="F8" s="4">
+        <v>0</v>
+      </c>
+      <c r="G8" s="4">
+        <v>11</v>
+      </c>
+      <c r="H8" s="4">
+        <v>0</v>
+      </c>
+      <c r="I8" s="4">
+        <v>0</v>
+      </c>
+      <c r="J8" s="4">
+        <v>7</v>
+      </c>
+      <c r="K8" s="6">
+        <f>SUM(B8:J8)</f>
+        <v>21</v>
+      </c>
+      <c r="L8" s="7">
+        <f>K8/COUNTIF(B8:J8, "&lt;&gt;")</f>
+        <v>2.3333333333333335</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="4">
+        <v>5</v>
+      </c>
+      <c r="C9" s="4">
+        <v>12</v>
+      </c>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="6">
+        <f>SUM(B9:J9)</f>
+        <v>17</v>
+      </c>
+      <c r="L9" s="7">
+        <f>K9/COUNTIF(B9:J9, "&lt;&gt;")</f>
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="4">
+        <v>0</v>
+      </c>
+      <c r="C10" s="4">
+        <v>0</v>
+      </c>
+      <c r="D10" s="4">
+        <v>12</v>
+      </c>
+      <c r="E10" s="4">
+        <v>3</v>
+      </c>
+      <c r="F10" s="4">
+        <v>0</v>
+      </c>
+      <c r="G10" s="4">
+        <v>0</v>
+      </c>
+      <c r="H10" s="4">
+        <v>0</v>
+      </c>
+      <c r="I10" s="4">
+        <v>0</v>
+      </c>
+      <c r="J10" s="4">
+        <v>0</v>
+      </c>
+      <c r="K10" s="6">
+        <f>SUM(B10:J10)</f>
         <v>15</v>
       </c>
-      <c r="B4" s="6">
-        <v>1</v>
-      </c>
-      <c r="C4" s="6">
+      <c r="L10" s="7">
+        <f>K10/COUNTIF(B10:J10, "&lt;&gt;")</f>
+        <v>1.6666666666666667</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A11" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="4">
+        <v>1</v>
+      </c>
+      <c r="C11" s="4">
+        <v>0</v>
+      </c>
+      <c r="D11" s="4">
+        <v>0</v>
+      </c>
+      <c r="E11" s="4">
+        <v>0</v>
+      </c>
+      <c r="F11" s="4">
+        <v>9</v>
+      </c>
+      <c r="G11" s="4">
+        <v>0</v>
+      </c>
+      <c r="H11" s="4">
+        <v>0</v>
+      </c>
+      <c r="I11" s="4">
+        <v>4</v>
+      </c>
+      <c r="J11" s="4">
+        <v>1</v>
+      </c>
+      <c r="K11" s="6">
+        <f>SUM(B11:J11)</f>
+        <v>15</v>
+      </c>
+      <c r="L11" s="7">
+        <f>K11/COUNTIF(B11:J11, "&lt;&gt;")</f>
+        <v>1.6666666666666667</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A12" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="4">
+        <v>5</v>
+      </c>
+      <c r="C12" s="4">
+        <v>0</v>
+      </c>
+      <c r="D12" s="4">
+        <v>1</v>
+      </c>
+      <c r="E12" s="4">
+        <v>3</v>
+      </c>
+      <c r="F12" s="4">
+        <v>3</v>
+      </c>
+      <c r="G12" s="4">
+        <v>2</v>
+      </c>
+      <c r="H12" s="4">
+        <v>1</v>
+      </c>
+      <c r="I12" s="4">
+        <v>0</v>
+      </c>
+      <c r="J12" s="4">
+        <v>0</v>
+      </c>
+      <c r="K12" s="6">
+        <f>SUM(B12:J12)</f>
+        <v>15</v>
+      </c>
+      <c r="L12" s="7">
+        <f>K12/COUNTIF(B12:J12, "&lt;&gt;")</f>
+        <v>1.6666666666666667</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A13" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="4">
+        <v>2</v>
+      </c>
+      <c r="C13" s="4">
+        <v>0</v>
+      </c>
+      <c r="D13" s="4">
+        <v>0</v>
+      </c>
+      <c r="E13" s="4">
+        <v>0</v>
+      </c>
+      <c r="F13" s="4">
+        <v>0</v>
+      </c>
+      <c r="G13" s="4">
+        <v>3</v>
+      </c>
+      <c r="H13" s="4">
+        <v>3</v>
+      </c>
+      <c r="I13" s="4">
+        <v>4</v>
+      </c>
+      <c r="J13" s="4">
+        <v>0</v>
+      </c>
+      <c r="K13" s="6">
+        <f>SUM(B13:J13)</f>
+        <v>12</v>
+      </c>
+      <c r="L13" s="7">
+        <f>K13/COUNTIF(B13:J13, "&lt;&gt;")</f>
+        <v>1.3333333333333333</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A14" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="4">
+        <v>0</v>
+      </c>
+      <c r="C14" s="4">
+        <v>0</v>
+      </c>
+      <c r="D14" s="4">
+        <v>0</v>
+      </c>
+      <c r="E14" s="4">
+        <v>0</v>
+      </c>
+      <c r="F14" s="4">
+        <v>3</v>
+      </c>
+      <c r="G14" s="4">
+        <v>2</v>
+      </c>
+      <c r="H14" s="4">
+        <v>0</v>
+      </c>
+      <c r="I14" s="4">
+        <v>0</v>
+      </c>
+      <c r="J14" s="4">
+        <v>7</v>
+      </c>
+      <c r="K14" s="6">
+        <f>SUM(B14:J14)</f>
+        <v>12</v>
+      </c>
+      <c r="L14" s="7">
+        <f>K14/COUNTIF(B14:J14, "&lt;&gt;")</f>
+        <v>1.3333333333333333</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A15" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" s="4">
+        <v>1</v>
+      </c>
+      <c r="C15" s="4">
+        <v>0</v>
+      </c>
+      <c r="D15" s="4">
+        <v>0</v>
+      </c>
+      <c r="E15" s="4">
+        <v>0</v>
+      </c>
+      <c r="F15" s="4">
+        <v>0</v>
+      </c>
+      <c r="G15" s="4">
+        <v>2</v>
+      </c>
+      <c r="H15" s="4">
+        <v>5</v>
+      </c>
+      <c r="I15" s="4">
+        <v>3</v>
+      </c>
+      <c r="J15" s="4">
+        <v>0</v>
+      </c>
+      <c r="K15" s="6">
+        <f>SUM(B15:J15)</f>
+        <v>11</v>
+      </c>
+      <c r="L15" s="7">
+        <f>K15/COUNTIF(B15:J15, "&lt;&gt;")</f>
+        <v>1.2222222222222223</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A16" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" s="4">
+        <v>5</v>
+      </c>
+      <c r="C16" s="4">
+        <v>3</v>
+      </c>
+      <c r="D16" s="4">
+        <v>0</v>
+      </c>
+      <c r="E16" s="4">
+        <v>0</v>
+      </c>
+      <c r="F16" s="4">
+        <v>2</v>
+      </c>
+      <c r="G16" s="4">
+        <v>0</v>
+      </c>
+      <c r="H16" s="4">
+        <v>0</v>
+      </c>
+      <c r="I16" s="4">
+        <v>0</v>
+      </c>
+      <c r="J16" s="4">
+        <v>1</v>
+      </c>
+      <c r="K16" s="6">
+        <f>SUM(B16:J16)</f>
+        <v>11</v>
+      </c>
+      <c r="L16" s="7">
+        <f>K16/COUNTIF(B16:J16, "&lt;&gt;")</f>
+        <v>1.2222222222222223</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A17" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="4">
+        <v>1</v>
+      </c>
+      <c r="C17" s="4">
+        <v>0</v>
+      </c>
+      <c r="D17" s="4">
+        <v>0</v>
+      </c>
+      <c r="E17" s="4">
+        <v>0</v>
+      </c>
+      <c r="F17" s="4">
+        <v>0</v>
+      </c>
+      <c r="G17" s="4">
+        <v>0</v>
+      </c>
+      <c r="H17" s="4">
+        <v>0</v>
+      </c>
+      <c r="I17" s="4">
+        <v>0</v>
+      </c>
+      <c r="J17" s="4">
+        <v>8</v>
+      </c>
+      <c r="K17" s="6">
+        <f>SUM(B17:J17)</f>
+        <v>9</v>
+      </c>
+      <c r="L17" s="7">
+        <f>K17/COUNTIF(B17:J17, "&lt;&gt;")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A18" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" s="4">
+        <v>1</v>
+      </c>
+      <c r="C18" s="4">
+        <v>0</v>
+      </c>
+      <c r="D18" s="4">
+        <v>3</v>
+      </c>
+      <c r="E18" s="4">
+        <v>3</v>
+      </c>
+      <c r="F18" s="4">
+        <v>1</v>
+      </c>
+      <c r="G18" s="4">
+        <v>0</v>
+      </c>
+      <c r="H18" s="4">
+        <v>0</v>
+      </c>
+      <c r="I18" s="4">
+        <v>0</v>
+      </c>
+      <c r="J18" s="4">
+        <v>0</v>
+      </c>
+      <c r="K18" s="6">
+        <f>SUM(B18:J18)</f>
+        <v>8</v>
+      </c>
+      <c r="L18" s="7">
+        <f>K18/COUNTIF(B18:J18, "&lt;&gt;")</f>
+        <v>0.88888888888888884</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A19" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" s="4">
         <v>6</v>
       </c>
-      <c r="D4" s="6">
-        <v>8</v>
-      </c>
-      <c r="E4" s="6">
-        <v>3</v>
-      </c>
-      <c r="F4" s="6">
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4"/>
+      <c r="K19" s="6">
+        <f>SUM(B19:J19)</f>
         <v>6</v>
       </c>
-      <c r="G4" s="6">
-        <v>3</v>
-      </c>
-      <c r="H4" s="6">
-        <v>0</v>
-      </c>
-      <c r="I4" s="6">
-        <v>0</v>
-      </c>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6">
-        <f t="shared" si="0"/>
-        <v>27</v>
-      </c>
-      <c r="L4" s="7">
-        <f>K4/COUNTIF(B4:I4, "&lt;&gt;")</f>
-        <v>3.375</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A5" s="9" t="s">
+      <c r="L19" s="7">
+        <f>K19/COUNTIF(B19:J19, "&lt;&gt;")</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A20" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" s="4">
+        <v>2</v>
+      </c>
+      <c r="C20" s="4">
+        <v>2</v>
+      </c>
+      <c r="D20" s="4">
+        <v>1</v>
+      </c>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4"/>
+      <c r="K20" s="6">
+        <f>SUM(B20:J20)</f>
         <v>5</v>
       </c>
-      <c r="B5" s="6">
-        <v>1</v>
-      </c>
-      <c r="C5" s="6">
-        <v>3</v>
-      </c>
-      <c r="D5" s="6">
+      <c r="L20" s="7">
+        <f>K20/COUNTIF(B20:J20, "&lt;&gt;")</f>
+        <v>1.6666666666666667</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A21" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21" s="4">
+        <v>3</v>
+      </c>
+      <c r="C21" s="4">
+        <v>0</v>
+      </c>
+      <c r="D21" s="4">
+        <v>0</v>
+      </c>
+      <c r="E21" s="4">
+        <v>0</v>
+      </c>
+      <c r="F21" s="4">
+        <v>0</v>
+      </c>
+      <c r="G21" s="4">
+        <v>1</v>
+      </c>
+      <c r="H21" s="4">
+        <v>0</v>
+      </c>
+      <c r="I21" s="4">
+        <v>0</v>
+      </c>
+      <c r="J21" s="4">
+        <v>0</v>
+      </c>
+      <c r="K21" s="6">
+        <f>SUM(B21:J21)</f>
         <v>4</v>
       </c>
-      <c r="E5" s="6">
-        <v>4</v>
-      </c>
-      <c r="F5" s="6">
-        <v>3</v>
-      </c>
-      <c r="G5" s="6">
-        <v>0</v>
-      </c>
-      <c r="H5" s="6">
-        <v>4</v>
-      </c>
-      <c r="I5" s="6">
-        <v>7</v>
-      </c>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6">
-        <f t="shared" si="0"/>
+      <c r="L21" s="7">
+        <f>K21/COUNTIF(B21:J21, "&lt;&gt;")</f>
+        <v>0.44444444444444442</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A22" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22" s="4">
+        <v>2</v>
+      </c>
+      <c r="C22" s="4">
+        <v>0</v>
+      </c>
+      <c r="D22" s="4">
+        <v>0</v>
+      </c>
+      <c r="E22" s="4">
+        <v>0</v>
+      </c>
+      <c r="F22" s="4">
+        <v>1</v>
+      </c>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="4"/>
+      <c r="K22" s="6">
+        <f>SUM(B22:J22)</f>
+        <v>3</v>
+      </c>
+      <c r="L22" s="7">
+        <f>K22/COUNTIF(B22:J22, "&lt;&gt;")</f>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A23" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23" s="4">
+        <v>0</v>
+      </c>
+      <c r="C23" s="4">
+        <v>0</v>
+      </c>
+      <c r="D23" s="4">
+        <v>0</v>
+      </c>
+      <c r="E23" s="4">
+        <v>0</v>
+      </c>
+      <c r="F23" s="4">
+        <v>0</v>
+      </c>
+      <c r="G23" s="4">
+        <v>1</v>
+      </c>
+      <c r="H23" s="4">
+        <v>0</v>
+      </c>
+      <c r="I23" s="4">
+        <v>0</v>
+      </c>
+      <c r="J23" s="4">
+        <v>0</v>
+      </c>
+      <c r="K23" s="6">
+        <f>SUM(B23:J23)</f>
+        <v>1</v>
+      </c>
+      <c r="L23" s="7">
+        <f>K23/COUNTIF(B23:J23, "&lt;&gt;")</f>
+        <v>0.1111111111111111</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A24" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B24" s="4">
+        <v>0</v>
+      </c>
+      <c r="C24" s="4">
+        <v>0</v>
+      </c>
+      <c r="D24" s="4">
+        <v>0</v>
+      </c>
+      <c r="E24" s="4">
+        <v>0</v>
+      </c>
+      <c r="F24" s="4">
+        <v>0</v>
+      </c>
+      <c r="G24" s="4">
+        <v>0</v>
+      </c>
+      <c r="H24" s="4"/>
+      <c r="I24" s="4"/>
+      <c r="J24" s="4"/>
+      <c r="K24" s="6">
+        <f>SUM(B24:J24)</f>
+        <v>0</v>
+      </c>
+      <c r="L24" s="7">
+        <f>K24/COUNTIF(B24:J24, "&lt;&gt;")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A25" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B25" s="4">
+        <v>0</v>
+      </c>
+      <c r="C25" s="4">
+        <v>0</v>
+      </c>
+      <c r="D25" s="4">
+        <v>0</v>
+      </c>
+      <c r="E25" s="4">
+        <v>0</v>
+      </c>
+      <c r="F25" s="4">
+        <v>0</v>
+      </c>
+      <c r="G25" s="4">
+        <v>0</v>
+      </c>
+      <c r="H25" s="4">
+        <v>0</v>
+      </c>
+      <c r="I25" s="4">
+        <v>0</v>
+      </c>
+      <c r="J25" s="4">
+        <v>0</v>
+      </c>
+      <c r="K25" s="6">
+        <f>SUM(B25:J25)</f>
+        <v>0</v>
+      </c>
+      <c r="L25" s="7">
+        <f>K25/COUNTIF(B25:J25, "&lt;&gt;")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A26" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="B26" s="11">
+        <v>56</v>
+      </c>
+      <c r="C26" s="11">
+        <v>44</v>
+      </c>
+      <c r="D26" s="11">
+        <v>47</v>
+      </c>
+      <c r="E26" s="11">
+        <v>36</v>
+      </c>
+      <c r="F26" s="11">
+        <v>36</v>
+      </c>
+      <c r="G26" s="11">
+        <v>41</v>
+      </c>
+      <c r="H26" s="11">
+        <v>28</v>
+      </c>
+      <c r="I26" s="11">
         <v>26</v>
       </c>
-      <c r="L5" s="7">
-        <f>K5/COUNTIF(B5:I5, "&lt;&gt;")</f>
-        <v>3.25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A6" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" s="6">
-        <v>8</v>
-      </c>
-      <c r="C6" s="6">
-        <v>9</v>
-      </c>
-      <c r="D6" s="6">
-        <v>4</v>
-      </c>
-      <c r="E6" s="6">
-        <v>0</v>
-      </c>
-      <c r="F6" s="6">
-        <v>0</v>
-      </c>
-      <c r="G6" s="6">
-        <v>0</v>
-      </c>
-      <c r="H6" s="6">
-        <v>2</v>
-      </c>
-      <c r="I6" s="6">
-        <v>2</v>
-      </c>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6">
-        <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-      <c r="L6" s="7">
-        <f>K6/COUNTIF(B6:I6, "&lt;&gt;")</f>
-        <v>3.125</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A7" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="6">
-        <v>6</v>
-      </c>
-      <c r="C7" s="6">
-        <v>4</v>
-      </c>
-      <c r="D7" s="6">
-        <v>0</v>
-      </c>
-      <c r="E7" s="6">
-        <v>0</v>
-      </c>
-      <c r="F7" s="6">
-        <v>0</v>
-      </c>
-      <c r="G7" s="6">
-        <v>0</v>
-      </c>
-      <c r="H7" s="6">
-        <v>9</v>
-      </c>
-      <c r="I7" s="6">
-        <v>2</v>
-      </c>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6">
-        <f t="shared" si="0"/>
-        <v>21</v>
-      </c>
-      <c r="L7" s="7">
-        <f>K7/COUNTIF(B7:I7, "&lt;&gt;")</f>
-        <v>2.625</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A8" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="6">
-        <v>5</v>
-      </c>
-      <c r="C8" s="6">
-        <v>12</v>
-      </c>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="6">
-        <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-      <c r="L8" s="7">
-        <f>K8/COUNTIF(B8:I8, "&lt;&gt;")</f>
-        <v>8.5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A9" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="6">
-        <v>0</v>
-      </c>
-      <c r="C9" s="6">
-        <v>0</v>
-      </c>
-      <c r="D9" s="6">
-        <v>12</v>
-      </c>
-      <c r="E9" s="6">
-        <v>3</v>
-      </c>
-      <c r="F9" s="6">
-        <v>0</v>
-      </c>
-      <c r="G9" s="6">
-        <v>0</v>
-      </c>
-      <c r="H9" s="6">
-        <v>0</v>
-      </c>
-      <c r="I9" s="6">
-        <v>0</v>
-      </c>
-      <c r="J9" s="6"/>
-      <c r="K9" s="6">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="L9" s="7">
-        <f>K9/COUNTIF(B9:I9, "&lt;&gt;")</f>
-        <v>1.875</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A10" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" s="6">
-        <v>5</v>
-      </c>
-      <c r="C10" s="6">
-        <v>0</v>
-      </c>
-      <c r="D10" s="6">
-        <v>1</v>
-      </c>
-      <c r="E10" s="6">
-        <v>3</v>
-      </c>
-      <c r="F10" s="6">
-        <v>3</v>
-      </c>
-      <c r="G10" s="6">
-        <v>2</v>
-      </c>
-      <c r="H10" s="6">
-        <v>1</v>
-      </c>
-      <c r="I10" s="6">
-        <v>0</v>
-      </c>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="L10" s="7">
-        <f>K10/COUNTIF(B10:I10, "&lt;&gt;")</f>
-        <v>1.875</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A11" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" s="6">
-        <v>1</v>
-      </c>
-      <c r="C11" s="6">
-        <v>0</v>
-      </c>
-      <c r="D11" s="6">
-        <v>0</v>
-      </c>
-      <c r="E11" s="6">
-        <v>2</v>
-      </c>
-      <c r="F11" s="6">
-        <v>0</v>
-      </c>
-      <c r="G11" s="6">
-        <v>11</v>
-      </c>
-      <c r="H11" s="6">
-        <v>0</v>
-      </c>
-      <c r="I11" s="6">
-        <v>0</v>
-      </c>
-      <c r="J11" s="6"/>
-      <c r="K11" s="6">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="L11" s="7">
-        <f>K11/COUNTIF(B11:I11, "&lt;&gt;")</f>
-        <v>1.75</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A12" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" s="6">
-        <v>1</v>
-      </c>
-      <c r="C12" s="6">
-        <v>0</v>
-      </c>
-      <c r="D12" s="6">
-        <v>0</v>
-      </c>
-      <c r="E12" s="6">
-        <v>0</v>
-      </c>
-      <c r="F12" s="6">
-        <v>9</v>
-      </c>
-      <c r="G12" s="6">
-        <v>0</v>
-      </c>
-      <c r="H12" s="6">
-        <v>0</v>
-      </c>
-      <c r="I12" s="6">
-        <v>4</v>
-      </c>
-      <c r="J12" s="6"/>
-      <c r="K12" s="6">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="L12" s="7">
-        <f>K12/COUNTIF(B12:I12, "&lt;&gt;")</f>
-        <v>1.75</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A13" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" s="6">
-        <v>2</v>
-      </c>
-      <c r="C13" s="6">
-        <v>0</v>
-      </c>
-      <c r="D13" s="6">
-        <v>0</v>
-      </c>
-      <c r="E13" s="6">
-        <v>0</v>
-      </c>
-      <c r="F13" s="6">
-        <v>0</v>
-      </c>
-      <c r="G13" s="6">
-        <v>3</v>
-      </c>
-      <c r="H13" s="6">
-        <v>3</v>
-      </c>
-      <c r="I13" s="6">
-        <v>4</v>
-      </c>
-      <c r="J13" s="6"/>
-      <c r="K13" s="6">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="L13" s="7">
-        <f>K13/COUNTIF(B13:I13, "&lt;&gt;")</f>
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A14" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="B14" s="6">
-        <v>1</v>
-      </c>
-      <c r="C14" s="6">
-        <v>0</v>
-      </c>
-      <c r="D14" s="6">
-        <v>0</v>
-      </c>
-      <c r="E14" s="6">
-        <v>0</v>
-      </c>
-      <c r="F14" s="6">
-        <v>0</v>
-      </c>
-      <c r="G14" s="6">
-        <v>2</v>
-      </c>
-      <c r="H14" s="6">
-        <v>5</v>
-      </c>
-      <c r="I14" s="6">
-        <v>3</v>
-      </c>
-      <c r="J14" s="6"/>
-      <c r="K14" s="6">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="L14" s="7">
-        <f>K14/COUNTIF(B14:I14, "&lt;&gt;")</f>
-        <v>1.375</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A15" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="B15" s="6">
-        <v>5</v>
-      </c>
-      <c r="C15" s="6">
-        <v>3</v>
-      </c>
-      <c r="D15" s="6">
-        <v>0</v>
-      </c>
-      <c r="E15" s="6">
-        <v>0</v>
-      </c>
-      <c r="F15" s="6">
-        <v>2</v>
-      </c>
-      <c r="G15" s="6">
-        <v>0</v>
-      </c>
-      <c r="H15" s="6">
-        <v>0</v>
-      </c>
-      <c r="I15" s="6">
-        <v>0</v>
-      </c>
-      <c r="J15" s="6"/>
-      <c r="K15" s="6">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="L15" s="7">
-        <f>K15/COUNTIF(B15:I15, "&lt;&gt;")</f>
-        <v>1.25</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A16" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B16" s="6">
-        <v>1</v>
-      </c>
-      <c r="C16" s="6">
-        <v>0</v>
-      </c>
-      <c r="D16" s="6">
-        <v>3</v>
-      </c>
-      <c r="E16" s="6">
-        <v>3</v>
-      </c>
-      <c r="F16" s="6">
-        <v>1</v>
-      </c>
-      <c r="G16" s="6">
-        <v>0</v>
-      </c>
-      <c r="H16" s="6">
-        <v>0</v>
-      </c>
-      <c r="I16" s="6">
-        <v>0</v>
-      </c>
-      <c r="J16" s="6"/>
-      <c r="K16" s="6">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="L16" s="7">
-        <f>K16/COUNTIF(B16:I16, "&lt;&gt;")</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A17" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B17" s="6">
-        <v>6</v>
-      </c>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="6"/>
-      <c r="J17" s="6"/>
-      <c r="K17" s="6">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="L17" s="7">
-        <f>K17/COUNTIF(B17:I17, "&lt;&gt;")</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A18" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="B18" s="6">
-        <v>0</v>
-      </c>
-      <c r="C18" s="6">
-        <v>0</v>
-      </c>
-      <c r="D18" s="6">
-        <v>0</v>
-      </c>
-      <c r="E18" s="6">
-        <v>0</v>
-      </c>
-      <c r="F18" s="6">
-        <v>3</v>
-      </c>
-      <c r="G18" s="6">
-        <v>2</v>
-      </c>
-      <c r="H18" s="6">
-        <v>0</v>
-      </c>
-      <c r="I18" s="6">
-        <v>0</v>
-      </c>
-      <c r="J18" s="6"/>
-      <c r="K18" s="6">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="L18" s="7">
-        <f>K18/COUNTIF(B18:I18, "&lt;&gt;")</f>
-        <v>0.625</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A19" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="B19" s="6">
-        <v>2</v>
-      </c>
-      <c r="C19" s="6">
-        <v>2</v>
-      </c>
-      <c r="D19" s="6">
-        <v>1</v>
-      </c>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
-      <c r="J19" s="6"/>
-      <c r="K19" s="6">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="L19" s="7">
-        <f>K19/COUNTIF(B19:I19, "&lt;&gt;")</f>
-        <v>1.6666666666666667</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A20" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B20" s="6">
-        <v>3</v>
-      </c>
-      <c r="C20" s="6">
-        <v>0</v>
-      </c>
-      <c r="D20" s="6">
-        <v>0</v>
-      </c>
-      <c r="E20" s="6">
-        <v>0</v>
-      </c>
-      <c r="F20" s="6">
-        <v>0</v>
-      </c>
-      <c r="G20" s="6">
-        <v>1</v>
-      </c>
-      <c r="H20" s="6">
-        <v>0</v>
-      </c>
-      <c r="I20" s="6">
-        <v>0</v>
-      </c>
-      <c r="J20" s="6"/>
-      <c r="K20" s="6">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="L20" s="7">
-        <f>K20/COUNTIF(B20:I20, "&lt;&gt;")</f>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A21" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B21" s="6">
-        <v>2</v>
-      </c>
-      <c r="C21" s="6">
-        <v>0</v>
-      </c>
-      <c r="D21" s="6">
-        <v>0</v>
-      </c>
-      <c r="E21" s="6">
-        <v>0</v>
-      </c>
-      <c r="F21" s="6">
-        <v>1</v>
-      </c>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
-      <c r="J21" s="6"/>
-      <c r="K21" s="6">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="L21" s="7">
-        <f>K21/COUNTIF(B21:I21, "&lt;&gt;")</f>
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A22" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B22" s="6">
-        <v>1</v>
-      </c>
-      <c r="C22" s="6">
-        <v>0</v>
-      </c>
-      <c r="D22" s="6">
-        <v>0</v>
-      </c>
-      <c r="E22" s="6">
-        <v>0</v>
-      </c>
-      <c r="F22" s="6">
-        <v>0</v>
-      </c>
-      <c r="G22" s="6">
-        <v>0</v>
-      </c>
-      <c r="H22" s="6">
-        <v>0</v>
-      </c>
-      <c r="I22" s="6">
-        <v>0</v>
-      </c>
-      <c r="J22" s="6"/>
-      <c r="K22" s="6">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="L22" s="7">
-        <f>K22/COUNTIF(B22:I22, "&lt;&gt;")</f>
-        <v>0.125</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A23" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="B23" s="6">
-        <v>0</v>
-      </c>
-      <c r="C23" s="6">
-        <v>0</v>
-      </c>
-      <c r="D23" s="6">
-        <v>0</v>
-      </c>
-      <c r="E23" s="6">
-        <v>0</v>
-      </c>
-      <c r="F23" s="6">
-        <v>0</v>
-      </c>
-      <c r="G23" s="6">
-        <v>1</v>
-      </c>
-      <c r="H23" s="6">
-        <v>0</v>
-      </c>
-      <c r="I23" s="6">
-        <v>0</v>
-      </c>
-      <c r="J23" s="6"/>
-      <c r="K23" s="6">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="L23" s="7">
-        <f>K23/COUNTIF(B23:I23, "&lt;&gt;")</f>
-        <v>0.125</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A24" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B24" s="6">
-        <v>0</v>
-      </c>
-      <c r="C24" s="6">
-        <v>0</v>
-      </c>
-      <c r="D24" s="6">
-        <v>0</v>
-      </c>
-      <c r="E24" s="6">
-        <v>0</v>
-      </c>
-      <c r="F24" s="6">
-        <v>0</v>
-      </c>
-      <c r="G24" s="6">
-        <v>0</v>
-      </c>
-      <c r="H24" s="6"/>
-      <c r="I24" s="6"/>
-      <c r="J24" s="6"/>
-      <c r="K24" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L24" s="7">
-        <f>K24/COUNTIF(B24:I24, "&lt;&gt;")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A25" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="B25" s="6">
-        <v>0</v>
-      </c>
-      <c r="C25" s="6">
-        <v>0</v>
-      </c>
-      <c r="D25" s="6">
-        <v>0</v>
-      </c>
-      <c r="E25" s="6">
-        <v>0</v>
-      </c>
-      <c r="F25" s="6">
-        <v>0</v>
-      </c>
-      <c r="G25" s="6">
-        <v>0</v>
-      </c>
-      <c r="H25" s="6">
-        <v>0</v>
-      </c>
-      <c r="I25" s="6">
-        <v>0</v>
-      </c>
-      <c r="J25" s="6"/>
-      <c r="K25" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L25" s="7">
-        <f>K25/COUNTIF(B25:I25, "&lt;&gt;")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A26" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="B26" s="12">
-        <v>56</v>
-      </c>
-      <c r="C26" s="12">
-        <v>44</v>
-      </c>
-      <c r="D26" s="12">
-        <v>47</v>
-      </c>
-      <c r="E26" s="12">
-        <v>36</v>
-      </c>
-      <c r="F26" s="12">
-        <v>36</v>
-      </c>
-      <c r="G26" s="12">
-        <v>41</v>
-      </c>
-      <c r="H26" s="12">
-        <v>28</v>
-      </c>
-      <c r="I26" s="12">
+      <c r="J26" s="11">
         <v>26</v>
       </c>
-      <c r="J26" s="12"/>
-      <c r="K26" s="12">
+      <c r="K26" s="11">
         <f>SUM(B26:J26)</f>
-        <v>314</v>
-      </c>
-      <c r="L26" s="13"/>
+        <v>340</v>
+      </c>
+      <c r="L26" s="12"/>
     </row>
     <row r="27" spans="1:12" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A27" s="14" t="s">
+      <c r="A27" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="B27" s="15">
+      <c r="B27" s="14">
         <f>B26/COUNTIF(B2:B25, "&lt;&gt;")</f>
         <v>2.3333333333333335</v>
       </c>
-      <c r="C27" s="15">
-        <f t="shared" ref="C27:I27" si="1">C26/COUNTIF(C2:C25, "&lt;&gt;")</f>
+      <c r="C27" s="14">
+        <f t="shared" ref="C27:I27" si="0">C26/COUNTIF(C2:C25, "&lt;&gt;")</f>
         <v>1.9130434782608696</v>
       </c>
-      <c r="D27" s="15">
-        <f t="shared" si="1"/>
+      <c r="D27" s="14">
+        <f t="shared" si="0"/>
         <v>2.1363636363636362</v>
       </c>
-      <c r="E27" s="15">
-        <f t="shared" si="1"/>
+      <c r="E27" s="14">
+        <f t="shared" si="0"/>
         <v>1.7142857142857142</v>
       </c>
-      <c r="F27" s="15">
-        <f t="shared" si="1"/>
+      <c r="F27" s="14">
+        <f t="shared" si="0"/>
         <v>1.7142857142857142</v>
       </c>
-      <c r="G27" s="15">
-        <f t="shared" si="1"/>
+      <c r="G27" s="14">
+        <f t="shared" si="0"/>
         <v>2.0499999999999998</v>
       </c>
-      <c r="H27" s="15">
-        <f t="shared" si="1"/>
+      <c r="H27" s="14">
+        <f t="shared" si="0"/>
         <v>1.4736842105263157</v>
       </c>
-      <c r="I27" s="15">
-        <f t="shared" si="1"/>
+      <c r="I27" s="14">
+        <f t="shared" si="0"/>
         <v>1.4444444444444444</v>
       </c>
-      <c r="J27" s="15"/>
-      <c r="K27" s="16"/>
-      <c r="L27" s="10"/>
+      <c r="J27" s="14"/>
+      <c r="K27" s="15"/>
+      <c r="L27" s="9"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L25">
     <sortCondition descending="1" ref="K2:K25"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
+  <conditionalFormatting sqref="K2:K25">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L2:L25">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
DAT updating conf data
</commit_message>
<xml_diff>
--- a/dev/data/survivor-au-confessionals.xlsx
+++ b/dev/data/survivor-au-confessionals.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dan\Google Drive\R Code\my-packages\survivoR\dev\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46058E94-96FF-4C67-936E-A8834589A7A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90E88F2B-7070-4203-906B-AC1C42CBF7B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" firstSheet="1" activeTab="1" xr2:uid="{22E0698C-8932-416E-AF95-78770299D9ED}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" firstSheet="1" activeTab="2" xr2:uid="{22E0698C-8932-416E-AF95-78770299D9ED}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="17" state="hidden" r:id="rId1"/>
@@ -22,7 +22,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="18" r:id="rId4"/>
+    <pivotCache cacheId="19" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -1969,7 +1969,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{63A8B301-3C2E-42ED-A9F3-C8CAD4EC449B}" name="PivotTable5" cacheId="18" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{63A8B301-3C2E-42ED-A9F3-C8CAD4EC449B}" name="PivotTable5" cacheId="19" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:K29" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField showAll="0"/>
@@ -3328,8 +3328,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{823259C0-A9B2-4D8C-810E-0A651DDDB32E}">
   <dimension ref="A1:F187"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView topLeftCell="A152" workbookViewId="0">
+      <selection activeCell="F181" sqref="F181"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -6979,7 +6979,7 @@
         <v>15</v>
       </c>
       <c r="F182">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="183" spans="1:6" x14ac:dyDescent="0.45">
@@ -7059,7 +7059,7 @@
         <v>7</v>
       </c>
       <c r="F186">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="187" spans="1:6" x14ac:dyDescent="0.45">
@@ -7096,8 +7096,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C07E9347-A5AE-4362-9039-760890A1C329}">
   <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -7172,11 +7172,11 @@
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
       <c r="K2" s="6">
-        <f>SUM(B2:J2)</f>
+        <f t="shared" ref="K2:K26" si="0">SUM(B2:J2)</f>
         <v>45</v>
       </c>
       <c r="L2" s="7">
-        <f>K2/COUNTIF(B2:J2, "&lt;&gt;")</f>
+        <f t="shared" ref="L2:L25" si="1">K2/COUNTIF(B2:J2, "&lt;&gt;")</f>
         <v>6.4285714285714288</v>
       </c>
     </row>
@@ -7209,15 +7209,15 @@
         <v>0</v>
       </c>
       <c r="J3" s="4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K3" s="6">
-        <f>SUM(B3:J3)</f>
-        <v>31</v>
+        <f t="shared" si="0"/>
+        <v>30</v>
       </c>
       <c r="L3" s="7">
-        <f>K3/COUNTIF(B3:J3, "&lt;&gt;")</f>
-        <v>3.4444444444444446</v>
+        <f t="shared" si="1"/>
+        <v>3.3333333333333335</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.45">
@@ -7252,11 +7252,11 @@
         <v>4</v>
       </c>
       <c r="K4" s="6">
-        <f>SUM(B4:J4)</f>
+        <f t="shared" si="0"/>
         <v>29</v>
       </c>
       <c r="L4" s="7">
-        <f>K4/COUNTIF(B4:J4, "&lt;&gt;")</f>
+        <f t="shared" si="1"/>
         <v>3.2222222222222223</v>
       </c>
     </row>
@@ -7292,11 +7292,11 @@
         <v>0</v>
       </c>
       <c r="K5" s="6">
-        <f>SUM(B5:J5)</f>
+        <f t="shared" si="0"/>
         <v>29</v>
       </c>
       <c r="L5" s="7">
-        <f>K5/COUNTIF(B5:J5, "&lt;&gt;")</f>
+        <f t="shared" si="1"/>
         <v>3.2222222222222223</v>
       </c>
     </row>
@@ -7329,15 +7329,15 @@
         <v>2</v>
       </c>
       <c r="J6" s="4">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K6" s="6">
-        <f>SUM(B6:J6)</f>
-        <v>28</v>
+        <f t="shared" si="0"/>
+        <v>27</v>
       </c>
       <c r="L6" s="7">
-        <f>K6/COUNTIF(B6:J6, "&lt;&gt;")</f>
-        <v>3.1111111111111112</v>
+        <f t="shared" si="1"/>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.45">
@@ -7372,11 +7372,11 @@
         <v>2</v>
       </c>
       <c r="K7" s="6">
-        <f>SUM(B7:J7)</f>
+        <f t="shared" si="0"/>
         <v>28</v>
       </c>
       <c r="L7" s="7">
-        <f>K7/COUNTIF(B7:J7, "&lt;&gt;")</f>
+        <f t="shared" si="1"/>
         <v>3.1111111111111112</v>
       </c>
     </row>
@@ -7412,11 +7412,11 @@
         <v>7</v>
       </c>
       <c r="K8" s="6">
-        <f>SUM(B8:J8)</f>
+        <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="L8" s="7">
-        <f>K8/COUNTIF(B8:J8, "&lt;&gt;")</f>
+        <f t="shared" si="1"/>
         <v>2.3333333333333335</v>
       </c>
     </row>
@@ -7438,11 +7438,11 @@
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
       <c r="K9" s="6">
-        <f>SUM(B9:J9)</f>
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="L9" s="7">
-        <f>K9/COUNTIF(B9:J9, "&lt;&gt;")</f>
+        <f t="shared" si="1"/>
         <v>8.5</v>
       </c>
     </row>
@@ -7478,11 +7478,11 @@
         <v>0</v>
       </c>
       <c r="K10" s="6">
-        <f>SUM(B10:J10)</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="L10" s="7">
-        <f>K10/COUNTIF(B10:J10, "&lt;&gt;")</f>
+        <f t="shared" si="1"/>
         <v>1.6666666666666667</v>
       </c>
     </row>
@@ -7518,11 +7518,11 @@
         <v>1</v>
       </c>
       <c r="K11" s="6">
-        <f>SUM(B11:J11)</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="L11" s="7">
-        <f>K11/COUNTIF(B11:J11, "&lt;&gt;")</f>
+        <f t="shared" si="1"/>
         <v>1.6666666666666667</v>
       </c>
     </row>
@@ -7558,11 +7558,11 @@
         <v>0</v>
       </c>
       <c r="K12" s="6">
-        <f>SUM(B12:J12)</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="L12" s="7">
-        <f>K12/COUNTIF(B12:J12, "&lt;&gt;")</f>
+        <f t="shared" si="1"/>
         <v>1.6666666666666667</v>
       </c>
     </row>
@@ -7598,11 +7598,11 @@
         <v>0</v>
       </c>
       <c r="K13" s="6">
-        <f>SUM(B13:J13)</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="L13" s="7">
-        <f>K13/COUNTIF(B13:J13, "&lt;&gt;")</f>
+        <f t="shared" si="1"/>
         <v>1.3333333333333333</v>
       </c>
     </row>
@@ -7638,11 +7638,11 @@
         <v>7</v>
       </c>
       <c r="K14" s="6">
-        <f>SUM(B14:J14)</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="L14" s="7">
-        <f>K14/COUNTIF(B14:J14, "&lt;&gt;")</f>
+        <f t="shared" si="1"/>
         <v>1.3333333333333333</v>
       </c>
     </row>
@@ -7678,11 +7678,11 @@
         <v>0</v>
       </c>
       <c r="K15" s="6">
-        <f>SUM(B15:J15)</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="L15" s="7">
-        <f>K15/COUNTIF(B15:J15, "&lt;&gt;")</f>
+        <f t="shared" si="1"/>
         <v>1.2222222222222223</v>
       </c>
     </row>
@@ -7718,11 +7718,11 @@
         <v>1</v>
       </c>
       <c r="K16" s="6">
-        <f>SUM(B16:J16)</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="L16" s="7">
-        <f>K16/COUNTIF(B16:J16, "&lt;&gt;")</f>
+        <f t="shared" si="1"/>
         <v>1.2222222222222223</v>
       </c>
     </row>
@@ -7758,11 +7758,11 @@
         <v>8</v>
       </c>
       <c r="K17" s="6">
-        <f>SUM(B17:J17)</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="L17" s="7">
-        <f>K17/COUNTIF(B17:J17, "&lt;&gt;")</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -7798,11 +7798,11 @@
         <v>0</v>
       </c>
       <c r="K18" s="6">
-        <f>SUM(B18:J18)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="L18" s="7">
-        <f>K18/COUNTIF(B18:J18, "&lt;&gt;")</f>
+        <f t="shared" si="1"/>
         <v>0.88888888888888884</v>
       </c>
     </row>
@@ -7822,11 +7822,11 @@
       <c r="I19" s="4"/>
       <c r="J19" s="4"/>
       <c r="K19" s="6">
-        <f>SUM(B19:J19)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="L19" s="7">
-        <f>K19/COUNTIF(B19:J19, "&lt;&gt;")</f>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
     </row>
@@ -7850,11 +7850,11 @@
       <c r="I20" s="4"/>
       <c r="J20" s="4"/>
       <c r="K20" s="6">
-        <f>SUM(B20:J20)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="L20" s="7">
-        <f>K20/COUNTIF(B20:J20, "&lt;&gt;")</f>
+        <f t="shared" si="1"/>
         <v>1.6666666666666667</v>
       </c>
     </row>
@@ -7890,11 +7890,11 @@
         <v>0</v>
       </c>
       <c r="K21" s="6">
-        <f>SUM(B21:J21)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="L21" s="7">
-        <f>K21/COUNTIF(B21:J21, "&lt;&gt;")</f>
+        <f t="shared" si="1"/>
         <v>0.44444444444444442</v>
       </c>
     </row>
@@ -7922,11 +7922,11 @@
       <c r="I22" s="4"/>
       <c r="J22" s="4"/>
       <c r="K22" s="6">
-        <f>SUM(B22:J22)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="L22" s="7">
-        <f>K22/COUNTIF(B22:J22, "&lt;&gt;")</f>
+        <f t="shared" si="1"/>
         <v>0.6</v>
       </c>
     </row>
@@ -7962,11 +7962,11 @@
         <v>0</v>
       </c>
       <c r="K23" s="6">
-        <f>SUM(B23:J23)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="L23" s="7">
-        <f>K23/COUNTIF(B23:J23, "&lt;&gt;")</f>
+        <f t="shared" si="1"/>
         <v>0.1111111111111111</v>
       </c>
     </row>
@@ -7996,11 +7996,11 @@
       <c r="I24" s="4"/>
       <c r="J24" s="4"/>
       <c r="K24" s="6">
-        <f>SUM(B24:J24)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L24" s="7">
-        <f>K24/COUNTIF(B24:J24, "&lt;&gt;")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -8036,11 +8036,11 @@
         <v>0</v>
       </c>
       <c r="K25" s="6">
-        <f>SUM(B25:J25)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L25" s="7">
-        <f>K25/COUNTIF(B25:J25, "&lt;&gt;")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -8076,7 +8076,7 @@
         <v>26</v>
       </c>
       <c r="K26" s="11">
-        <f>SUM(B26:J26)</f>
+        <f t="shared" si="0"/>
         <v>340</v>
       </c>
       <c r="L26" s="12"/>
@@ -8090,31 +8090,31 @@
         <v>2.3333333333333335</v>
       </c>
       <c r="C27" s="14">
-        <f t="shared" ref="C27:I27" si="0">C26/COUNTIF(C2:C25, "&lt;&gt;")</f>
+        <f t="shared" ref="C27:I27" si="2">C26/COUNTIF(C2:C25, "&lt;&gt;")</f>
         <v>1.9130434782608696</v>
       </c>
       <c r="D27" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2.1363636363636362</v>
       </c>
       <c r="E27" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.7142857142857142</v>
       </c>
       <c r="F27" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.7142857142857142</v>
       </c>
       <c r="G27" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2.0499999999999998</v>
       </c>
       <c r="H27" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.4736842105263157</v>
       </c>
       <c r="I27" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.4444444444444444</v>
       </c>
       <c r="J27" s="14"/>

</xml_diff>

<commit_message>
DEV update to confessionals
</commit_message>
<xml_diff>
--- a/dev/data/survivor-au-confessionals.xlsx
+++ b/dev/data/survivor-au-confessionals.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dan\Google Drive\R Code\my-packages\survivoR\dev\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D5DDED7-69BD-4AE0-88C1-B9E45F348909}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4170949B-F8EC-454B-89E0-D46BFDF01E41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" firstSheet="1" activeTab="2" xr2:uid="{22E0698C-8932-416E-AF95-78770299D9ED}"/>
   </bookViews>
@@ -19,10 +19,11 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Confessionals!$A$1:$F$70</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Table!$A$1:$O$27</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="20" r:id="rId4"/>
+    <pivotCache cacheId="3" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="727" uniqueCount="74">
   <si>
     <t>Sandra</t>
   </si>
@@ -259,6 +260,12 @@
   <si>
     <t>Boot order</t>
   </si>
+  <si>
+    <t>Episode 10</t>
+  </si>
+  <si>
+    <t>Episode 11</t>
+  </si>
 </sst>
 </file>
 
@@ -411,9 +418,9 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Daniel Oehm" refreshedDate="44607.971429050929" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" recordCount="186" xr:uid="{09B81C42-1F32-493D-A094-1828F2ECB888}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Daniel Oehm" refreshedDate="44614.552690509256" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" recordCount="217" xr:uid="{C0C5FE16-3602-4240-B470-E73A3D9FDB7E}">
   <cacheSource type="worksheet">
-    <worksheetSource ref="A1:F187" sheet="Confessionals"/>
+    <worksheetSource ref="A1:F218" sheet="Confessionals"/>
   </cacheSource>
   <cacheFields count="6">
     <cacheField name="Season Name" numFmtId="0">
@@ -423,7 +430,7 @@
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="7" maxValue="7"/>
     </cacheField>
     <cacheField name="Episode" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="9" count="9">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="11" count="11">
         <n v="1"/>
         <n v="2"/>
         <n v="3"/>
@@ -433,6 +440,8 @@
         <n v="7"/>
         <n v="8"/>
         <n v="9"/>
+        <n v="10"/>
+        <n v="11"/>
       </sharedItems>
     </cacheField>
     <cacheField name="Castaway ID" numFmtId="0">
@@ -467,7 +476,7 @@
       </sharedItems>
     </cacheField>
     <cacheField name="Confessional Count" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="14"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="16"/>
     </cacheField>
   </cacheFields>
   <extLst>
@@ -479,7 +488,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="186">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="217">
   <r>
     <s v="Survivor: Blood V. Water"/>
     <n v="7"/>
@@ -1926,7 +1935,7 @@
     <x v="8"/>
     <s v="AU0019"/>
     <x v="14"/>
-    <n v="4"/>
+    <n v="3"/>
   </r>
   <r>
     <s v="Survivor: Blood V. Water"/>
@@ -1958,7 +1967,7 @@
     <x v="8"/>
     <s v="AU0023"/>
     <x v="19"/>
-    <n v="7"/>
+    <n v="6"/>
   </r>
   <r>
     <s v="Survivor: Blood V. Water"/>
@@ -1968,17 +1977,265 @@
     <x v="22"/>
     <n v="1"/>
   </r>
+  <r>
+    <s v="Survivor: Blood V. Water"/>
+    <n v="7"/>
+    <x v="9"/>
+    <s v="AU0002"/>
+    <x v="3"/>
+    <n v="4"/>
+  </r>
+  <r>
+    <s v="Survivor: Blood V. Water"/>
+    <n v="7"/>
+    <x v="9"/>
+    <s v="AU0003"/>
+    <x v="6"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <s v="Survivor: Blood V. Water"/>
+    <n v="7"/>
+    <x v="9"/>
+    <s v="AU0004"/>
+    <x v="7"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <s v="Survivor: Blood V. Water"/>
+    <n v="7"/>
+    <x v="9"/>
+    <s v="AU0006"/>
+    <x v="9"/>
+    <n v="16"/>
+  </r>
+  <r>
+    <s v="Survivor: Blood V. Water"/>
+    <n v="7"/>
+    <x v="9"/>
+    <s v="AU0007"/>
+    <x v="10"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <s v="Survivor: Blood V. Water"/>
+    <n v="7"/>
+    <x v="9"/>
+    <s v="AU0009"/>
+    <x v="18"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <s v="Survivor: Blood V. Water"/>
+    <n v="7"/>
+    <x v="9"/>
+    <s v="AU0010"/>
+    <x v="20"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <s v="Survivor: Blood V. Water"/>
+    <n v="7"/>
+    <x v="9"/>
+    <s v="AU0016"/>
+    <x v="5"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <s v="Survivor: Blood V. Water"/>
+    <n v="7"/>
+    <x v="9"/>
+    <s v="AU0017"/>
+    <x v="11"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <s v="Survivor: Blood V. Water"/>
+    <n v="7"/>
+    <x v="9"/>
+    <s v="AU0018"/>
+    <x v="12"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <s v="Survivor: Blood V. Water"/>
+    <n v="7"/>
+    <x v="9"/>
+    <s v="AU0019"/>
+    <x v="14"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <s v="Survivor: Blood V. Water"/>
+    <n v="7"/>
+    <x v="9"/>
+    <s v="AU0020"/>
+    <x v="15"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <s v="Survivor: Blood V. Water"/>
+    <n v="7"/>
+    <x v="9"/>
+    <s v="AU0021"/>
+    <x v="16"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <s v="Survivor: Blood V. Water"/>
+    <n v="7"/>
+    <x v="9"/>
+    <s v="AU0022"/>
+    <x v="17"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <s v="Survivor: Blood V. Water"/>
+    <n v="7"/>
+    <x v="9"/>
+    <s v="AU0023"/>
+    <x v="19"/>
+    <n v="8"/>
+  </r>
+  <r>
+    <s v="Survivor: Blood V. Water"/>
+    <n v="7"/>
+    <x v="9"/>
+    <s v="AU0024"/>
+    <x v="22"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <s v="Survivor: Blood V. Water"/>
+    <n v="7"/>
+    <x v="10"/>
+    <s v="AU0004"/>
+    <x v="7"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <s v="Survivor: Blood V. Water"/>
+    <n v="7"/>
+    <x v="10"/>
+    <s v="AU0007"/>
+    <x v="10"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <s v="Survivor: Blood V. Water"/>
+    <n v="7"/>
+    <x v="10"/>
+    <s v="AU0017"/>
+    <x v="11"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <s v="Survivor: Blood V. Water"/>
+    <n v="7"/>
+    <x v="10"/>
+    <s v="AU0018"/>
+    <x v="12"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <s v="Survivor: Blood V. Water"/>
+    <n v="7"/>
+    <x v="10"/>
+    <s v="AU0021"/>
+    <x v="16"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <s v="Survivor: Blood V. Water"/>
+    <n v="7"/>
+    <x v="10"/>
+    <s v="AU0022"/>
+    <x v="17"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <s v="Survivor: Blood V. Water"/>
+    <n v="7"/>
+    <x v="10"/>
+    <s v="AU0024"/>
+    <x v="22"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <s v="Survivor: Blood V. Water"/>
+    <n v="7"/>
+    <x v="10"/>
+    <s v="AU0002"/>
+    <x v="3"/>
+    <n v="5"/>
+  </r>
+  <r>
+    <s v="Survivor: Blood V. Water"/>
+    <n v="7"/>
+    <x v="10"/>
+    <s v="AU0003"/>
+    <x v="6"/>
+    <n v="5"/>
+  </r>
+  <r>
+    <s v="Survivor: Blood V. Water"/>
+    <n v="7"/>
+    <x v="10"/>
+    <s v="AU0006"/>
+    <x v="9"/>
+    <n v="4"/>
+  </r>
+  <r>
+    <s v="Survivor: Blood V. Water"/>
+    <n v="7"/>
+    <x v="10"/>
+    <s v="AU0009"/>
+    <x v="18"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <s v="Survivor: Blood V. Water"/>
+    <n v="7"/>
+    <x v="10"/>
+    <s v="AU0010"/>
+    <x v="20"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <s v="Survivor: Blood V. Water"/>
+    <n v="7"/>
+    <x v="10"/>
+    <s v="AU0016"/>
+    <x v="5"/>
+    <n v="5"/>
+  </r>
+  <r>
+    <s v="Survivor: Blood V. Water"/>
+    <n v="7"/>
+    <x v="10"/>
+    <s v="AU0019"/>
+    <x v="14"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <s v="Survivor: Blood V. Water"/>
+    <n v="7"/>
+    <x v="10"/>
+    <s v="AU0020"/>
+    <x v="15"/>
+    <n v="5"/>
+  </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{63A8B301-3C2E-42ED-A9F3-C8CAD4EC449B}" name="PivotTable5" cacheId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A3:K29" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{887622D4-D2D5-4521-90C2-945890A5BC22}" name="PivotTable5" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:M29" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField axis="axisCol" showAll="0">
-      <items count="10">
+      <items count="12">
         <item x="0"/>
         <item x="1"/>
         <item x="2"/>
@@ -1988,6 +2245,8 @@
         <item x="6"/>
         <item x="7"/>
         <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -2106,7 +2365,7 @@
   <colFields count="1">
     <field x="2"/>
   </colFields>
-  <colItems count="10">
+  <colItems count="12">
     <i>
       <x/>
     </i>
@@ -2133,6 +2392,12 @@
     </i>
     <i>
       <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="10"/>
     </i>
     <i t="grand">
       <x/>
@@ -2450,21 +2715,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F537B13A-F125-4516-AC8E-0BC38A122EBA}">
-  <dimension ref="A3:K29"/>
+  <dimension ref="A3:M29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:J28"/>
+      <selection activeCell="B5" sqref="B5:L28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="22.796875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.73046875" bestFit="1" customWidth="1"/>
-    <col min="3" max="10" width="2.73046875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.19921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="12" width="2.73046875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>58</v>
       </c>
@@ -2472,7 +2737,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>55</v>
       </c>
@@ -2503,11 +2768,17 @@
       <c r="J4">
         <v>9</v>
       </c>
-      <c r="K4" t="s">
+      <c r="K4">
+        <v>10</v>
+      </c>
+      <c r="L4">
+        <v>11</v>
+      </c>
+      <c r="M4" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A5" s="3" t="s">
         <v>9</v>
       </c>
@@ -2530,11 +2801,13 @@
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
-      <c r="K5" s="4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A6" s="3" t="s">
         <v>16</v>
       </c>
@@ -2565,11 +2838,13 @@
       <c r="J6" s="4">
         <v>7</v>
       </c>
-      <c r="K6" s="4">
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4">
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A7" s="3" t="s">
         <v>4</v>
       </c>
@@ -2584,11 +2859,13 @@
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
-      <c r="K7" s="4">
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A8" s="3" t="s">
         <v>8</v>
       </c>
@@ -2620,10 +2897,16 @@
         <v>0</v>
       </c>
       <c r="K8" s="4">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
+        <v>4</v>
+      </c>
+      <c r="L8" s="4">
+        <v>5</v>
+      </c>
+      <c r="M8" s="4">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A9" s="3" t="s">
         <v>10</v>
       </c>
@@ -2640,11 +2923,13 @@
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
-      <c r="K9" s="4">
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A10" s="3" t="s">
         <v>18</v>
       </c>
@@ -2676,10 +2961,16 @@
         <v>4</v>
       </c>
       <c r="K10" s="4">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
+        <v>1</v>
+      </c>
+      <c r="L10" s="4">
+        <v>5</v>
+      </c>
+      <c r="M10" s="4">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A11" s="3" t="s">
         <v>17</v>
       </c>
@@ -2711,10 +3002,16 @@
         <v>0</v>
       </c>
       <c r="K11" s="4">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
+        <v>1</v>
+      </c>
+      <c r="L11" s="4">
+        <v>5</v>
+      </c>
+      <c r="M11" s="4">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A12" s="3" t="s">
         <v>6</v>
       </c>
@@ -2746,10 +3043,16 @@
         <v>0</v>
       </c>
       <c r="K12" s="4">
+        <v>0</v>
+      </c>
+      <c r="L12" s="4">
+        <v>0</v>
+      </c>
+      <c r="M12" s="4">
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A13" s="3" t="s">
         <v>12</v>
       </c>
@@ -2774,11 +3077,13 @@
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
-      <c r="K13" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="K13" s="4"/>
+      <c r="L13" s="4"/>
+      <c r="M13" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A14" s="3" t="s">
         <v>11</v>
       </c>
@@ -2810,10 +3115,16 @@
         <v>0</v>
       </c>
       <c r="K14" s="4">
+        <v>16</v>
+      </c>
+      <c r="L14" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="M14" s="4">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A15" s="3" t="s">
         <v>21</v>
       </c>
@@ -2845,10 +3156,16 @@
         <v>7</v>
       </c>
       <c r="K15" s="4">
+        <v>0</v>
+      </c>
+      <c r="L15" s="4">
+        <v>0</v>
+      </c>
+      <c r="M15" s="4">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A16" s="3" t="s">
         <v>22</v>
       </c>
@@ -2880,10 +3197,16 @@
         <v>0</v>
       </c>
       <c r="K16" s="4">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
+        <v>2</v>
+      </c>
+      <c r="L16" s="4">
+        <v>0</v>
+      </c>
+      <c r="M16" s="4">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A17" s="3" t="s">
         <v>13</v>
       </c>
@@ -2915,10 +3238,16 @@
         <v>8</v>
       </c>
       <c r="K17" s="4">
+        <v>0</v>
+      </c>
+      <c r="L17" s="4">
+        <v>0</v>
+      </c>
+      <c r="M17" s="4">
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A18" s="3" t="s">
         <v>20</v>
       </c>
@@ -2937,11 +3266,13 @@
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
       <c r="J18" s="4"/>
-      <c r="K18" s="4">
+      <c r="K18" s="4"/>
+      <c r="L18" s="4"/>
+      <c r="M18" s="4">
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A19" s="3" t="s">
         <v>15</v>
       </c>
@@ -2970,13 +3301,19 @@
         <v>0</v>
       </c>
       <c r="J19" s="4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K19" s="4">
+        <v>1</v>
+      </c>
+      <c r="L19" s="4">
+        <v>0</v>
+      </c>
+      <c r="M19" s="4">
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A20" s="3" t="s">
         <v>14</v>
       </c>
@@ -3008,10 +3345,16 @@
         <v>1</v>
       </c>
       <c r="K20" s="4">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
+        <v>1</v>
+      </c>
+      <c r="L20" s="4">
+        <v>5</v>
+      </c>
+      <c r="M20" s="4">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A21" s="3" t="s">
         <v>23</v>
       </c>
@@ -3043,10 +3386,16 @@
         <v>0</v>
       </c>
       <c r="K21" s="4">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.45">
+        <v>3</v>
+      </c>
+      <c r="L21" s="4">
+        <v>0</v>
+      </c>
+      <c r="M21" s="4">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A22" s="3" t="s">
         <v>19</v>
       </c>
@@ -3080,8 +3429,14 @@
       <c r="K22" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L22" s="4">
+        <v>0</v>
+      </c>
+      <c r="M22" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A23" s="3" t="s">
         <v>3</v>
       </c>
@@ -3113,10 +3468,16 @@
         <v>0</v>
       </c>
       <c r="K23" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.45">
+        <v>0</v>
+      </c>
+      <c r="L23" s="4">
+        <v>0</v>
+      </c>
+      <c r="M23" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A24" s="3" t="s">
         <v>7</v>
       </c>
@@ -3145,13 +3506,17 @@
         <v>2</v>
       </c>
       <c r="J24" s="4">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K24" s="4">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.45">
+        <v>8</v>
+      </c>
+      <c r="L24" s="4"/>
+      <c r="M24" s="4">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A25" s="3" t="s">
         <v>5</v>
       </c>
@@ -3183,10 +3548,16 @@
         <v>2</v>
       </c>
       <c r="K25" s="4">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.45">
+        <v>1</v>
+      </c>
+      <c r="L25" s="4">
+        <v>1</v>
+      </c>
+      <c r="M25" s="4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A26" s="3" t="s">
         <v>0</v>
       </c>
@@ -3213,11 +3584,13 @@
       </c>
       <c r="I26" s="4"/>
       <c r="J26" s="4"/>
-      <c r="K26" s="4">
+      <c r="K26" s="4"/>
+      <c r="L26" s="4"/>
+      <c r="M26" s="4">
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A27" s="3" t="s">
         <v>1</v>
       </c>
@@ -3249,10 +3622,16 @@
         <v>1</v>
       </c>
       <c r="K27" s="4">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.45">
+        <v>0</v>
+      </c>
+      <c r="L27" s="4">
+        <v>3</v>
+      </c>
+      <c r="M27" s="4">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A28" s="3" t="s">
         <v>2</v>
       </c>
@@ -3283,11 +3662,13 @@
       <c r="J28" s="4">
         <v>0</v>
       </c>
-      <c r="K28" s="4">
+      <c r="K28" s="4"/>
+      <c r="L28" s="4"/>
+      <c r="M28" s="4">
         <v>29</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A29" s="3" t="s">
         <v>56</v>
       </c>
@@ -3316,10 +3697,16 @@
         <v>26</v>
       </c>
       <c r="J29" s="4">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="K29" s="4">
-        <v>355</v>
+        <v>38</v>
+      </c>
+      <c r="L29" s="4">
+        <v>28</v>
+      </c>
+      <c r="M29" s="4">
+        <v>419</v>
       </c>
     </row>
   </sheetData>
@@ -3329,10 +3716,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{823259C0-A9B2-4D8C-810E-0A651DDDB32E}">
-  <dimension ref="A1:F187"/>
+  <dimension ref="A1:F218"/>
   <sheetViews>
-    <sheetView topLeftCell="A152" workbookViewId="0">
-      <selection activeCell="F181" sqref="F181"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D218" sqref="D218"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -7085,6 +7472,626 @@
         <v>1</v>
       </c>
     </row>
+    <row r="188" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A188" t="s">
+        <v>52</v>
+      </c>
+      <c r="B188">
+        <v>7</v>
+      </c>
+      <c r="C188">
+        <v>10</v>
+      </c>
+      <c r="D188" t="s">
+        <v>29</v>
+      </c>
+      <c r="E188" t="s">
+        <v>8</v>
+      </c>
+      <c r="F188">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="189" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A189" t="s">
+        <v>52</v>
+      </c>
+      <c r="B189">
+        <v>7</v>
+      </c>
+      <c r="C189">
+        <v>10</v>
+      </c>
+      <c r="D189" t="s">
+        <v>30</v>
+      </c>
+      <c r="E189" t="s">
+        <v>17</v>
+      </c>
+      <c r="F189">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="190" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A190" t="s">
+        <v>52</v>
+      </c>
+      <c r="B190">
+        <v>7</v>
+      </c>
+      <c r="C190">
+        <v>10</v>
+      </c>
+      <c r="D190" t="s">
+        <v>31</v>
+      </c>
+      <c r="E190" t="s">
+        <v>6</v>
+      </c>
+      <c r="F190">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="191" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A191" t="s">
+        <v>52</v>
+      </c>
+      <c r="B191">
+        <v>7</v>
+      </c>
+      <c r="C191">
+        <v>10</v>
+      </c>
+      <c r="D191" t="s">
+        <v>33</v>
+      </c>
+      <c r="E191" t="s">
+        <v>11</v>
+      </c>
+      <c r="F191">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="192" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A192" t="s">
+        <v>52</v>
+      </c>
+      <c r="B192">
+        <v>7</v>
+      </c>
+      <c r="C192">
+        <v>10</v>
+      </c>
+      <c r="D192" t="s">
+        <v>34</v>
+      </c>
+      <c r="E192" t="s">
+        <v>21</v>
+      </c>
+      <c r="F192">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="193" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A193" t="s">
+        <v>52</v>
+      </c>
+      <c r="B193">
+        <v>7</v>
+      </c>
+      <c r="C193">
+        <v>10</v>
+      </c>
+      <c r="D193" t="s">
+        <v>36</v>
+      </c>
+      <c r="E193" t="s">
+        <v>3</v>
+      </c>
+      <c r="F193">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="194" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A194" t="s">
+        <v>52</v>
+      </c>
+      <c r="B194">
+        <v>7</v>
+      </c>
+      <c r="C194">
+        <v>10</v>
+      </c>
+      <c r="D194" t="s">
+        <v>37</v>
+      </c>
+      <c r="E194" t="s">
+        <v>5</v>
+      </c>
+      <c r="F194">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="195" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A195" t="s">
+        <v>52</v>
+      </c>
+      <c r="B195">
+        <v>7</v>
+      </c>
+      <c r="C195">
+        <v>10</v>
+      </c>
+      <c r="D195" t="s">
+        <v>43</v>
+      </c>
+      <c r="E195" t="s">
+        <v>18</v>
+      </c>
+      <c r="F195">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="196" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A196" t="s">
+        <v>52</v>
+      </c>
+      <c r="B196">
+        <v>7</v>
+      </c>
+      <c r="C196">
+        <v>10</v>
+      </c>
+      <c r="D196" t="s">
+        <v>44</v>
+      </c>
+      <c r="E196" t="s">
+        <v>22</v>
+      </c>
+      <c r="F196">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="197" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A197" t="s">
+        <v>52</v>
+      </c>
+      <c r="B197">
+        <v>7</v>
+      </c>
+      <c r="C197">
+        <v>10</v>
+      </c>
+      <c r="D197" t="s">
+        <v>45</v>
+      </c>
+      <c r="E197" t="s">
+        <v>13</v>
+      </c>
+      <c r="F197">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="198" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A198" t="s">
+        <v>52</v>
+      </c>
+      <c r="B198">
+        <v>7</v>
+      </c>
+      <c r="C198">
+        <v>10</v>
+      </c>
+      <c r="D198" t="s">
+        <v>46</v>
+      </c>
+      <c r="E198" t="s">
+        <v>15</v>
+      </c>
+      <c r="F198">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="199" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A199" t="s">
+        <v>52</v>
+      </c>
+      <c r="B199">
+        <v>7</v>
+      </c>
+      <c r="C199">
+        <v>10</v>
+      </c>
+      <c r="D199" t="s">
+        <v>47</v>
+      </c>
+      <c r="E199" t="s">
+        <v>14</v>
+      </c>
+      <c r="F199">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="200" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A200" t="s">
+        <v>52</v>
+      </c>
+      <c r="B200">
+        <v>7</v>
+      </c>
+      <c r="C200">
+        <v>10</v>
+      </c>
+      <c r="D200" t="s">
+        <v>48</v>
+      </c>
+      <c r="E200" t="s">
+        <v>23</v>
+      </c>
+      <c r="F200">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="201" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A201" t="s">
+        <v>52</v>
+      </c>
+      <c r="B201">
+        <v>7</v>
+      </c>
+      <c r="C201">
+        <v>10</v>
+      </c>
+      <c r="D201" t="s">
+        <v>49</v>
+      </c>
+      <c r="E201" t="s">
+        <v>19</v>
+      </c>
+      <c r="F201">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="202" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A202" t="s">
+        <v>52</v>
+      </c>
+      <c r="B202">
+        <v>7</v>
+      </c>
+      <c r="C202">
+        <v>10</v>
+      </c>
+      <c r="D202" t="s">
+        <v>50</v>
+      </c>
+      <c r="E202" t="s">
+        <v>7</v>
+      </c>
+      <c r="F202">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="203" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A203" t="s">
+        <v>52</v>
+      </c>
+      <c r="B203">
+        <v>7</v>
+      </c>
+      <c r="C203">
+        <v>10</v>
+      </c>
+      <c r="D203" t="s">
+        <v>51</v>
+      </c>
+      <c r="E203" t="s">
+        <v>1</v>
+      </c>
+      <c r="F203">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="204" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A204" t="s">
+        <v>52</v>
+      </c>
+      <c r="B204">
+        <v>7</v>
+      </c>
+      <c r="C204">
+        <v>11</v>
+      </c>
+      <c r="D204" t="s">
+        <v>31</v>
+      </c>
+      <c r="E204" t="s">
+        <v>6</v>
+      </c>
+      <c r="F204">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="205" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A205" t="s">
+        <v>52</v>
+      </c>
+      <c r="B205">
+        <v>7</v>
+      </c>
+      <c r="C205">
+        <v>11</v>
+      </c>
+      <c r="D205" t="s">
+        <v>34</v>
+      </c>
+      <c r="E205" t="s">
+        <v>21</v>
+      </c>
+      <c r="F205">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="206" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A206" t="s">
+        <v>52</v>
+      </c>
+      <c r="B206">
+        <v>7</v>
+      </c>
+      <c r="C206">
+        <v>11</v>
+      </c>
+      <c r="D206" t="s">
+        <v>44</v>
+      </c>
+      <c r="E206" t="s">
+        <v>22</v>
+      </c>
+      <c r="F206">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="207" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A207" t="s">
+        <v>52</v>
+      </c>
+      <c r="B207">
+        <v>7</v>
+      </c>
+      <c r="C207">
+        <v>11</v>
+      </c>
+      <c r="D207" t="s">
+        <v>45</v>
+      </c>
+      <c r="E207" t="s">
+        <v>13</v>
+      </c>
+      <c r="F207">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="208" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A208" t="s">
+        <v>52</v>
+      </c>
+      <c r="B208">
+        <v>7</v>
+      </c>
+      <c r="C208">
+        <v>11</v>
+      </c>
+      <c r="D208" t="s">
+        <v>48</v>
+      </c>
+      <c r="E208" t="s">
+        <v>23</v>
+      </c>
+      <c r="F208">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="209" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A209" t="s">
+        <v>52</v>
+      </c>
+      <c r="B209">
+        <v>7</v>
+      </c>
+      <c r="C209">
+        <v>11</v>
+      </c>
+      <c r="D209" t="s">
+        <v>49</v>
+      </c>
+      <c r="E209" t="s">
+        <v>19</v>
+      </c>
+      <c r="F209">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="210" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A210" t="s">
+        <v>52</v>
+      </c>
+      <c r="B210">
+        <v>7</v>
+      </c>
+      <c r="C210">
+        <v>11</v>
+      </c>
+      <c r="D210" t="s">
+        <v>51</v>
+      </c>
+      <c r="E210" t="s">
+        <v>1</v>
+      </c>
+      <c r="F210">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="211" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A211" t="s">
+        <v>52</v>
+      </c>
+      <c r="B211">
+        <v>7</v>
+      </c>
+      <c r="C211">
+        <v>11</v>
+      </c>
+      <c r="D211" t="s">
+        <v>29</v>
+      </c>
+      <c r="E211" t="s">
+        <v>8</v>
+      </c>
+      <c r="F211">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="212" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A212" t="s">
+        <v>52</v>
+      </c>
+      <c r="B212">
+        <v>7</v>
+      </c>
+      <c r="C212">
+        <v>11</v>
+      </c>
+      <c r="D212" t="s">
+        <v>30</v>
+      </c>
+      <c r="E212" t="s">
+        <v>17</v>
+      </c>
+      <c r="F212">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="213" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A213" t="s">
+        <v>52</v>
+      </c>
+      <c r="B213">
+        <v>7</v>
+      </c>
+      <c r="C213">
+        <v>11</v>
+      </c>
+      <c r="D213" t="s">
+        <v>33</v>
+      </c>
+      <c r="E213" t="s">
+        <v>11</v>
+      </c>
+      <c r="F213">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="214" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A214" t="s">
+        <v>52</v>
+      </c>
+      <c r="B214">
+        <v>7</v>
+      </c>
+      <c r="C214">
+        <v>11</v>
+      </c>
+      <c r="D214" t="s">
+        <v>36</v>
+      </c>
+      <c r="E214" t="s">
+        <v>3</v>
+      </c>
+      <c r="F214">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="215" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A215" t="s">
+        <v>52</v>
+      </c>
+      <c r="B215">
+        <v>7</v>
+      </c>
+      <c r="C215">
+        <v>11</v>
+      </c>
+      <c r="D215" t="s">
+        <v>37</v>
+      </c>
+      <c r="E215" t="s">
+        <v>5</v>
+      </c>
+      <c r="F215">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="216" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A216" t="s">
+        <v>52</v>
+      </c>
+      <c r="B216">
+        <v>7</v>
+      </c>
+      <c r="C216">
+        <v>11</v>
+      </c>
+      <c r="D216" t="s">
+        <v>43</v>
+      </c>
+      <c r="E216" t="s">
+        <v>18</v>
+      </c>
+      <c r="F216">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="217" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A217" t="s">
+        <v>52</v>
+      </c>
+      <c r="B217">
+        <v>7</v>
+      </c>
+      <c r="C217">
+        <v>11</v>
+      </c>
+      <c r="D217" t="s">
+        <v>46</v>
+      </c>
+      <c r="E217" t="s">
+        <v>15</v>
+      </c>
+      <c r="F217">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="218" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A218" t="s">
+        <v>52</v>
+      </c>
+      <c r="B218">
+        <v>7</v>
+      </c>
+      <c r="C218">
+        <v>11</v>
+      </c>
+      <c r="D218" t="s">
+        <v>47</v>
+      </c>
+      <c r="E218" t="s">
+        <v>14</v>
+      </c>
+      <c r="F218">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:F70" xr:uid="{823259C0-A9B2-4D8C-810E-0A651DDDB32E}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F70">
@@ -7097,20 +8104,22 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C07E9347-A5AE-4362-9039-760890A1C329}">
-  <dimension ref="A1:M27"/>
+  <dimension ref="A1:O27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="12.86328125" customWidth="1"/>
     <col min="2" max="2" width="6.73046875" customWidth="1"/>
-    <col min="3" max="12" width="9.06640625" style="5"/>
+    <col min="3" max="11" width="9.06640625" style="5"/>
+    <col min="12" max="13" width="10" style="5" customWidth="1"/>
+    <col min="14" max="14" width="9.06640625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="33.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:15" ht="33.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="8" t="s">
         <v>27</v>
       </c>
@@ -7145,13 +8154,19 @@
         <v>70</v>
       </c>
       <c r="L1" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="M1" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="N1" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="O1" s="8" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
         <v>15</v>
       </c>
@@ -7183,16 +8198,22 @@
       <c r="K2" s="4">
         <v>3</v>
       </c>
-      <c r="L2" s="6">
-        <f>SUM(C2:K2)</f>
-        <v>30</v>
-      </c>
-      <c r="M2" s="7">
-        <f>L2/COUNTIF(C2:K2, "&lt;&gt;")</f>
-        <v>3.3333333333333335</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="L2" s="4">
+        <v>1</v>
+      </c>
+      <c r="M2" s="4">
+        <v>0</v>
+      </c>
+      <c r="N2" s="6">
+        <f>SUM(C2:M2)</f>
+        <v>31</v>
+      </c>
+      <c r="O2" s="7">
+        <f>N2/COUNTIF(C2:M2, "&lt;&gt;")</f>
+        <v>2.8181818181818183</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
         <v>18</v>
       </c>
@@ -7224,16 +8245,22 @@
       <c r="K3" s="4">
         <v>4</v>
       </c>
-      <c r="L3" s="6">
-        <f>SUM(C3:K3)</f>
-        <v>29</v>
-      </c>
-      <c r="M3" s="7">
-        <f>L3/COUNTIF(C3:K3, "&lt;&gt;")</f>
-        <v>3.2222222222222223</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="L3" s="4">
+        <v>1</v>
+      </c>
+      <c r="M3" s="4">
+        <v>5</v>
+      </c>
+      <c r="N3" s="6">
+        <f t="shared" ref="N3:N25" si="0">SUM(C3:M3)</f>
+        <v>35</v>
+      </c>
+      <c r="O3" s="7">
+        <f t="shared" ref="O3:O25" si="1">N3/COUNTIF(C3:M3, "&lt;&gt;")</f>
+        <v>3.1818181818181817</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
@@ -7265,31 +8292,37 @@
       <c r="K4" s="4">
         <v>2</v>
       </c>
-      <c r="L4" s="6">
-        <f>SUM(C4:K4)</f>
-        <v>28</v>
-      </c>
-      <c r="M4" s="7">
-        <f>L4/COUNTIF(C4:K4, "&lt;&gt;")</f>
-        <v>3.1111111111111112</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="L4" s="4">
+        <v>1</v>
+      </c>
+      <c r="M4" s="4">
+        <v>1</v>
+      </c>
+      <c r="N4" s="6">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="O4" s="7">
+        <f t="shared" si="1"/>
+        <v>2.7272727272727271</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A5" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="4">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D5" s="4">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E5" s="4">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="F5" s="4">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G5" s="4">
         <v>0</v>
@@ -7298,42 +8331,48 @@
         <v>0</v>
       </c>
       <c r="I5" s="4">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="J5" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K5" s="4">
-        <v>6</v>
-      </c>
-      <c r="L5" s="6">
-        <f>SUM(C5:K5)</f>
-        <v>27</v>
-      </c>
-      <c r="M5" s="7">
-        <f>L5/COUNTIF(C5:K5, "&lt;&gt;")</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
+        <v>0</v>
+      </c>
+      <c r="L5" s="4">
+        <v>0</v>
+      </c>
+      <c r="M5" s="4">
+        <v>0</v>
+      </c>
+      <c r="N5" s="6">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="O5" s="7">
+        <f t="shared" si="1"/>
+        <v>1.3636363636363635</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A6" s="3" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6" s="4">
         <v>0</v>
       </c>
       <c r="E6" s="4">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="F6" s="4">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G6" s="4">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="H6" s="4">
         <v>0</v>
@@ -7342,77 +8381,89 @@
         <v>0</v>
       </c>
       <c r="J6" s="4">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K6" s="4">
-        <v>0</v>
-      </c>
-      <c r="L6" s="6">
-        <f>SUM(C6:K6)</f>
-        <v>15</v>
-      </c>
-      <c r="M6" s="7">
-        <f>L6/COUNTIF(C6:K6, "&lt;&gt;")</f>
-        <v>1.6666666666666667</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
+        <v>1</v>
+      </c>
+      <c r="L6" s="4">
+        <v>1</v>
+      </c>
+      <c r="M6" s="4">
+        <v>5</v>
+      </c>
+      <c r="N6" s="6">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="O6" s="7">
+        <f t="shared" si="1"/>
+        <v>1.9090909090909092</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A7" s="3" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="4">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D7" s="4">
         <v>0</v>
       </c>
       <c r="E7" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F7" s="4">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G7" s="4">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="H7" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I7" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J7" s="4">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="K7" s="4">
-        <v>1</v>
-      </c>
-      <c r="L7" s="6">
-        <f>SUM(C7:K7)</f>
-        <v>15</v>
-      </c>
-      <c r="M7" s="7">
-        <f>L7/COUNTIF(C7:K7, "&lt;&gt;")</f>
-        <v>1.6666666666666667</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
+        <v>0</v>
+      </c>
+      <c r="L7" s="4">
+        <v>3</v>
+      </c>
+      <c r="M7" s="4">
+        <v>0</v>
+      </c>
+      <c r="N7" s="6">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="O7" s="7">
+        <f t="shared" si="1"/>
+        <v>1.6363636363636365</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A8" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="4">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D8" s="4">
         <v>0</v>
       </c>
       <c r="E8" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F8" s="4">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G8" s="4">
         <v>3</v>
@@ -7421,74 +8472,86 @@
         <v>2</v>
       </c>
       <c r="I8" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J8" s="4">
         <v>0</v>
       </c>
       <c r="K8" s="4">
-        <v>0</v>
-      </c>
-      <c r="L8" s="6">
-        <f>SUM(C8:K8)</f>
-        <v>15</v>
-      </c>
-      <c r="M8" s="7">
-        <f>L8/COUNTIF(C8:K8, "&lt;&gt;")</f>
-        <v>1.6666666666666667</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
+        <v>7</v>
+      </c>
+      <c r="L8" s="4">
+        <v>0</v>
+      </c>
+      <c r="M8" s="4">
+        <v>0</v>
+      </c>
+      <c r="N8" s="6">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="O8" s="7">
+        <f t="shared" si="1"/>
+        <v>1.0909090909090908</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A9" s="3" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="4">
+        <v>1</v>
+      </c>
+      <c r="D9" s="4">
+        <v>0</v>
+      </c>
+      <c r="E9" s="4">
+        <v>0</v>
+      </c>
+      <c r="F9" s="4">
+        <v>0</v>
+      </c>
+      <c r="G9" s="4">
+        <v>0</v>
+      </c>
+      <c r="H9" s="4">
         <v>2</v>
       </c>
-      <c r="D9" s="4">
-        <v>0</v>
-      </c>
-      <c r="E9" s="4">
-        <v>0</v>
-      </c>
-      <c r="F9" s="4">
-        <v>0</v>
-      </c>
-      <c r="G9" s="4">
-        <v>0</v>
-      </c>
-      <c r="H9" s="4">
-        <v>3</v>
-      </c>
       <c r="I9" s="4">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="J9" s="4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K9" s="4">
         <v>0</v>
       </c>
-      <c r="L9" s="6">
-        <f>SUM(C9:K9)</f>
-        <v>12</v>
-      </c>
-      <c r="M9" s="7">
-        <f>L9/COUNTIF(C9:K9, "&lt;&gt;")</f>
-        <v>1.3333333333333333</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="L9" s="4">
+        <v>2</v>
+      </c>
+      <c r="M9" s="4">
+        <v>0</v>
+      </c>
+      <c r="N9" s="6">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="O9" s="7">
+        <f t="shared" si="1"/>
+        <v>1.1818181818181819</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A10" s="3" t="s">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="4">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D10" s="4">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E10" s="4">
         <v>0</v>
@@ -7497,10 +8560,10 @@
         <v>0</v>
       </c>
       <c r="G10" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H10" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I10" s="4">
         <v>0</v>
@@ -7509,20 +8572,26 @@
         <v>0</v>
       </c>
       <c r="K10" s="4">
-        <v>7</v>
-      </c>
-      <c r="L10" s="6">
-        <f>SUM(C10:K10)</f>
-        <v>12</v>
-      </c>
-      <c r="M10" s="7">
-        <f>L10/COUNTIF(C10:K10, "&lt;&gt;")</f>
-        <v>1.3333333333333333</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
+        <v>1</v>
+      </c>
+      <c r="L10" s="4">
+        <v>0</v>
+      </c>
+      <c r="M10" s="4">
+        <v>3</v>
+      </c>
+      <c r="N10" s="6">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="O10" s="7">
+        <f t="shared" si="1"/>
+        <v>1.2727272727272727</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A11" s="3" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="4">
@@ -7541,74 +8610,86 @@
         <v>0</v>
       </c>
       <c r="H11" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I11" s="4">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="J11" s="4">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K11" s="4">
-        <v>0</v>
-      </c>
-      <c r="L11" s="6">
-        <f>SUM(C11:K11)</f>
-        <v>11</v>
-      </c>
-      <c r="M11" s="7">
-        <f>L11/COUNTIF(C11:K11, "&lt;&gt;")</f>
-        <v>1.2222222222222223</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
+        <v>8</v>
+      </c>
+      <c r="L11" s="4">
+        <v>0</v>
+      </c>
+      <c r="M11" s="4">
+        <v>0</v>
+      </c>
+      <c r="N11" s="6">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="O11" s="7">
+        <f t="shared" si="1"/>
+        <v>0.81818181818181823</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A12" s="3" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="4">
+        <v>1</v>
+      </c>
+      <c r="D12" s="4">
+        <v>0</v>
+      </c>
+      <c r="E12" s="4">
+        <v>3</v>
+      </c>
+      <c r="F12" s="4">
+        <v>3</v>
+      </c>
+      <c r="G12" s="4">
+        <v>1</v>
+      </c>
+      <c r="H12" s="4">
+        <v>0</v>
+      </c>
+      <c r="I12" s="4">
+        <v>0</v>
+      </c>
+      <c r="J12" s="4">
+        <v>0</v>
+      </c>
+      <c r="K12" s="4">
+        <v>0</v>
+      </c>
+      <c r="L12" s="4">
+        <v>4</v>
+      </c>
+      <c r="M12" s="4">
         <v>5</v>
       </c>
-      <c r="D12" s="4">
-        <v>3</v>
-      </c>
-      <c r="E12" s="4">
-        <v>0</v>
-      </c>
-      <c r="F12" s="4">
-        <v>0</v>
-      </c>
-      <c r="G12" s="4">
-        <v>2</v>
-      </c>
-      <c r="H12" s="4">
-        <v>0</v>
-      </c>
-      <c r="I12" s="4">
-        <v>0</v>
-      </c>
-      <c r="J12" s="4">
-        <v>0</v>
-      </c>
-      <c r="K12" s="4">
-        <v>1</v>
-      </c>
-      <c r="L12" s="6">
-        <f>SUM(C12:K12)</f>
+      <c r="N12" s="6">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="O12" s="7">
+        <f t="shared" si="1"/>
+        <v>1.5454545454545454</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A13" s="3" t="s">
         <v>11</v>
-      </c>
-      <c r="M12" s="7">
-        <f>L12/COUNTIF(C12:K12, "&lt;&gt;")</f>
-        <v>1.2222222222222223</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A13" s="3" t="s">
-        <v>13</v>
       </c>
       <c r="B13" s="3"/>
       <c r="C13" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D13" s="4">
         <v>0</v>
@@ -7623,7 +8704,7 @@
         <v>0</v>
       </c>
       <c r="H13" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I13" s="4">
         <v>0</v>
@@ -7632,39 +8713,45 @@
         <v>0</v>
       </c>
       <c r="K13" s="4">
-        <v>8</v>
-      </c>
-      <c r="L13" s="6">
-        <f>SUM(C13:K13)</f>
-        <v>9</v>
-      </c>
-      <c r="M13" s="7">
-        <f>L13/COUNTIF(C13:K13, "&lt;&gt;")</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
+        <v>0</v>
+      </c>
+      <c r="L13" s="4">
+        <v>16</v>
+      </c>
+      <c r="M13" s="4">
+        <v>4</v>
+      </c>
+      <c r="N13" s="6">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="O13" s="7">
+        <f t="shared" si="1"/>
+        <v>2.1818181818181817</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A14" s="3" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D14" s="4">
         <v>0</v>
       </c>
       <c r="E14" s="4">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F14" s="4">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G14" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H14" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I14" s="4">
         <v>0</v>
@@ -7675,22 +8762,28 @@
       <c r="K14" s="4">
         <v>0</v>
       </c>
-      <c r="L14" s="6">
-        <f>SUM(C14:K14)</f>
-        <v>8</v>
-      </c>
-      <c r="M14" s="7">
-        <f>L14/COUNTIF(C14:K14, "&lt;&gt;")</f>
-        <v>0.88888888888888884</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="L14" s="4">
+        <v>0</v>
+      </c>
+      <c r="M14" s="4">
+        <v>0</v>
+      </c>
+      <c r="N14" s="6">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="O14" s="7">
+        <f t="shared" si="1"/>
+        <v>9.0909090909090912E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A15" s="3" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="B15" s="3"/>
       <c r="C15" s="4">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D15" s="4">
         <v>0</v>
@@ -7705,7 +8798,7 @@
         <v>0</v>
       </c>
       <c r="H15" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I15" s="4">
         <v>0</v>
@@ -7716,66 +8809,82 @@
       <c r="K15" s="4">
         <v>0</v>
       </c>
-      <c r="L15" s="6">
-        <f>SUM(C15:K15)</f>
+      <c r="L15" s="4">
+        <v>0</v>
+      </c>
+      <c r="M15" s="4">
+        <v>0</v>
+      </c>
+      <c r="N15" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O15" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A16" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="3">
+        <v>11</v>
+      </c>
+      <c r="C16" s="4">
+        <v>2</v>
+      </c>
+      <c r="D16" s="4">
+        <v>0</v>
+      </c>
+      <c r="E16" s="4">
+        <v>0</v>
+      </c>
+      <c r="F16" s="4">
+        <v>0</v>
+      </c>
+      <c r="G16" s="4">
+        <v>0</v>
+      </c>
+      <c r="H16" s="4">
+        <v>3</v>
+      </c>
+      <c r="I16" s="4">
+        <v>3</v>
+      </c>
+      <c r="J16" s="4">
         <v>4</v>
       </c>
-      <c r="M15" s="7">
-        <f>L15/COUNTIF(C15:K15, "&lt;&gt;")</f>
-        <v>0.44444444444444442</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A16" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="4">
-        <v>0</v>
-      </c>
-      <c r="D16" s="4">
-        <v>0</v>
-      </c>
-      <c r="E16" s="4">
-        <v>0</v>
-      </c>
-      <c r="F16" s="4">
-        <v>0</v>
-      </c>
-      <c r="G16" s="4">
-        <v>0</v>
-      </c>
-      <c r="H16" s="4">
-        <v>1</v>
-      </c>
-      <c r="I16" s="4">
-        <v>0</v>
-      </c>
-      <c r="J16" s="4">
-        <v>0</v>
-      </c>
       <c r="K16" s="4">
         <v>0</v>
       </c>
-      <c r="L16" s="6">
-        <f>SUM(C16:K16)</f>
-        <v>1</v>
-      </c>
-      <c r="M16" s="7">
-        <f>L16/COUNTIF(C16:K16, "&lt;&gt;")</f>
-        <v>0.1111111111111111</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="L16" s="4">
+        <v>1</v>
+      </c>
+      <c r="M16" s="4">
+        <v>5</v>
+      </c>
+      <c r="N16" s="6">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="O16" s="7">
+        <f t="shared" si="1"/>
+        <v>1.6363636363636365</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A17" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B17" s="3"/>
+        <v>7</v>
+      </c>
+      <c r="B17" s="3">
+        <v>10</v>
+      </c>
       <c r="C17" s="4">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D17" s="4">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E17" s="4">
         <v>0</v>
@@ -7790,24 +8899,28 @@
         <v>0</v>
       </c>
       <c r="I17" s="4">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="J17" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K17" s="4">
-        <v>0</v>
-      </c>
-      <c r="L17" s="6">
-        <f>SUM(C17:K17)</f>
-        <v>0</v>
-      </c>
-      <c r="M17" s="7">
-        <f>L17/COUNTIF(C17:K17, "&lt;&gt;")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.45">
+        <v>6</v>
+      </c>
+      <c r="L17" s="4">
+        <v>8</v>
+      </c>
+      <c r="M17" s="4"/>
+      <c r="N17" s="6">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="O17" s="7">
+        <f t="shared" si="1"/>
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A18" s="3" t="s">
         <v>16</v>
       </c>
@@ -7841,16 +8954,18 @@
       <c r="K18" s="4">
         <v>7</v>
       </c>
-      <c r="L18" s="6">
-        <f>SUM(C18:K18)</f>
+      <c r="L18" s="4"/>
+      <c r="M18" s="4"/>
+      <c r="N18" s="6">
+        <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="M18" s="7">
-        <f>L18/COUNTIF(C18:K18, "&lt;&gt;")</f>
+      <c r="O18" s="7">
+        <f t="shared" si="1"/>
         <v>2.3333333333333335</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A19" s="3" t="s">
         <v>2</v>
       </c>
@@ -7884,16 +8999,18 @@
       <c r="K19" s="4">
         <v>0</v>
       </c>
-      <c r="L19" s="6">
-        <f>SUM(C19:K19)</f>
+      <c r="L19" s="4"/>
+      <c r="M19" s="4"/>
+      <c r="N19" s="6">
+        <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="M19" s="7">
-        <f>L19/COUNTIF(C19:K19, "&lt;&gt;")</f>
+      <c r="O19" s="7">
+        <f t="shared" si="1"/>
         <v>3.2222222222222223</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A20" s="3" t="s">
         <v>0</v>
       </c>
@@ -7923,16 +9040,18 @@
       </c>
       <c r="J20" s="4"/>
       <c r="K20" s="4"/>
-      <c r="L20" s="6">
-        <f>SUM(C20:K20)</f>
+      <c r="L20" s="4"/>
+      <c r="M20" s="4"/>
+      <c r="N20" s="6">
+        <f t="shared" si="0"/>
         <v>45</v>
       </c>
-      <c r="M20" s="7">
-        <f>L20/COUNTIF(C20:K20, "&lt;&gt;")</f>
+      <c r="O20" s="7">
+        <f t="shared" si="1"/>
         <v>6.4285714285714288</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A21" s="3" t="s">
         <v>12</v>
       </c>
@@ -7960,16 +9079,18 @@
       <c r="I21" s="4"/>
       <c r="J21" s="4"/>
       <c r="K21" s="4"/>
-      <c r="L21" s="6">
-        <f>SUM(C21:K21)</f>
-        <v>0</v>
-      </c>
-      <c r="M21" s="7">
-        <f>L21/COUNTIF(C21:K21, "&lt;&gt;")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="L21" s="4"/>
+      <c r="M21" s="4"/>
+      <c r="N21" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O21" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A22" s="3" t="s">
         <v>9</v>
       </c>
@@ -7995,16 +9116,18 @@
       <c r="I22" s="4"/>
       <c r="J22" s="4"/>
       <c r="K22" s="4"/>
-      <c r="L22" s="6">
-        <f>SUM(C22:K22)</f>
-        <v>3</v>
-      </c>
-      <c r="M22" s="7">
-        <f>L22/COUNTIF(C22:K22, "&lt;&gt;")</f>
+      <c r="L22" s="4"/>
+      <c r="M22" s="4"/>
+      <c r="N22" s="6">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="O22" s="7">
+        <f t="shared" si="1"/>
         <v>0.6</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A23" s="3" t="s">
         <v>20</v>
       </c>
@@ -8026,16 +9149,18 @@
       <c r="I23" s="4"/>
       <c r="J23" s="4"/>
       <c r="K23" s="4"/>
-      <c r="L23" s="6">
-        <f>SUM(C23:K23)</f>
+      <c r="L23" s="4"/>
+      <c r="M23" s="4"/>
+      <c r="N23" s="6">
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="M23" s="7">
-        <f>L23/COUNTIF(C23:K23, "&lt;&gt;")</f>
+      <c r="O23" s="7">
+        <f t="shared" si="1"/>
         <v>1.6666666666666667</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A24" s="3" t="s">
         <v>10</v>
       </c>
@@ -8055,16 +9180,18 @@
       <c r="I24" s="4"/>
       <c r="J24" s="4"/>
       <c r="K24" s="4"/>
-      <c r="L24" s="6">
-        <f>SUM(C24:K24)</f>
+      <c r="L24" s="4"/>
+      <c r="M24" s="4"/>
+      <c r="N24" s="6">
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="M24" s="7">
-        <f>L24/COUNTIF(C24:K24, "&lt;&gt;")</f>
+      <c r="O24" s="7">
+        <f t="shared" si="1"/>
         <v>8.5</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A25" s="3" t="s">
         <v>4</v>
       </c>
@@ -8082,54 +9209,73 @@
       <c r="I25" s="4"/>
       <c r="J25" s="4"/>
       <c r="K25" s="4"/>
-      <c r="L25" s="6">
-        <f>SUM(C25:K25)</f>
+      <c r="L25" s="4"/>
+      <c r="M25" s="4"/>
+      <c r="N25" s="6">
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="M25" s="7">
-        <f>L25/COUNTIF(C25:K25, "&lt;&gt;")</f>
+      <c r="O25" s="7">
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A26" s="10" t="s">
         <v>67</v>
       </c>
       <c r="B26" s="10"/>
       <c r="C26" s="11">
+        <f>SUM(C2:C25)</f>
         <v>56</v>
       </c>
       <c r="D26" s="11">
+        <f t="shared" ref="D26:M26" si="2">SUM(D2:D25)</f>
         <v>44</v>
       </c>
       <c r="E26" s="11">
+        <f t="shared" si="2"/>
         <v>47</v>
       </c>
       <c r="F26" s="11">
+        <f t="shared" si="2"/>
         <v>36</v>
       </c>
       <c r="G26" s="11">
+        <f t="shared" si="2"/>
         <v>36</v>
       </c>
       <c r="H26" s="11">
+        <f t="shared" si="2"/>
         <v>41</v>
       </c>
       <c r="I26" s="11">
+        <f t="shared" si="2"/>
         <v>28</v>
       </c>
       <c r="J26" s="11">
+        <f t="shared" si="2"/>
         <v>26</v>
       </c>
       <c r="K26" s="11">
-        <v>26</v>
+        <f t="shared" si="2"/>
+        <v>39</v>
       </c>
       <c r="L26" s="11">
-        <f>SUM(C26:K26)</f>
-        <v>340</v>
-      </c>
-      <c r="M26" s="12"/>
-    </row>
-    <row r="27" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+        <f t="shared" si="2"/>
+        <v>38</v>
+      </c>
+      <c r="M26" s="11">
+        <f t="shared" si="2"/>
+        <v>28</v>
+      </c>
+      <c r="N26" s="11">
+        <f>SUM(C26:M26)</f>
+        <v>419</v>
+      </c>
+      <c r="O26" s="12"/>
+    </row>
+    <row r="27" spans="1:15" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A27" s="13" t="s">
         <v>69</v>
       </c>
@@ -8166,17 +9312,28 @@
         <f>J26/COUNTIF(J2:J25, "&lt;&gt;")</f>
         <v>1.4444444444444444</v>
       </c>
-      <c r="K27" s="14"/>
-      <c r="L27" s="15"/>
-      <c r="M27" s="9"/>
+      <c r="K27" s="14">
+        <f t="shared" ref="K27:M27" si="3">K26/COUNTIF(K2:K25, "&lt;&gt;")</f>
+        <v>2.1666666666666665</v>
+      </c>
+      <c r="L27" s="14">
+        <f t="shared" si="3"/>
+        <v>2.375</v>
+      </c>
+      <c r="M27" s="14">
+        <f t="shared" si="3"/>
+        <v>1.8666666666666667</v>
+      </c>
+      <c r="N27" s="15"/>
+      <c r="O27" s="9"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M27">
-    <sortCondition descending="1" ref="B2:B27"/>
-    <sortCondition descending="1" ref="L2:L27"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O25">
+    <sortCondition descending="1" ref="B2:B25"/>
+    <sortCondition descending="1" ref="N2:N25"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="L2:L25">
+  <conditionalFormatting sqref="N2:N25">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -8186,7 +9343,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M2:M25">
+  <conditionalFormatting sqref="O2:O25">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -8199,7 +9356,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="L2:M25" formulaRange="1"/>
+    <ignoredError sqref="O2:O25 N2:N25" formulaRange="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>